<commit_message>
Added more user IDs for user stories
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steam\Documents\__INFO310\SubscriptionTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4293508A-560F-40B7-BF74-A73210270B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A75795-30EC-4D33-823C-B60DB8302C98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="7" r:id="rId1"/>
@@ -1472,15 +1472,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1508,6 +1499,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1515,9 +1515,29 @@
   <dxfs count="28">
     <dxf>
       <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1603,29 +1623,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3976,13 +3976,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1051560</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>323850</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4014,14 +4014,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4169,13 +4169,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2305050</xdr:colOff>
+          <xdr:colOff>2308860</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4207,14 +4207,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4238,13 +4238,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2590800</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4276,14 +4276,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4350,13 +4350,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>1981200</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4388,14 +4388,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4419,13 +4419,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2286000</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>251460</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4457,14 +4457,14 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -4839,25 +4839,25 @@
       <selection activeCell="A14" sqref="A14:IV14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="59.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="256" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="59.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
@@ -4885,7 +4885,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="G4" s="47"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2</v>
       </c>
@@ -4933,7 +4933,7 @@
       <c r="G5" s="48"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="40"/>
       <c r="C6" s="22" t="str">
@@ -4952,7 +4952,7 @@
       <c r="G6" s="48"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="40"/>
       <c r="C7" s="22" t="str">
@@ -4971,7 +4971,7 @@
       <c r="G7" s="48"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="40"/>
       <c r="C8" s="22" t="str">
@@ -4990,7 +4990,7 @@
       <c r="G8" s="48"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="40"/>
       <c r="C9" s="22" t="str">
@@ -5009,7 +5009,7 @@
       <c r="G9" s="48"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="41"/>
       <c r="C10" s="42" t="str">
@@ -5028,17 +5028,17 @@
       <c r="G10" s="49"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -5068,7 +5068,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>1</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>2</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>3</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>4</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>5</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <v>6</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="str">
         <f t="shared" ref="A22:A30" si="3">IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),A21+1,"")</f>
         <v/>
@@ -5277,7 +5277,7 @@
       <c r="H22" s="29"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5303,7 +5303,7 @@
       <c r="H23" s="29"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5329,7 +5329,7 @@
       <c r="H24" s="29"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5355,7 +5355,7 @@
       <c r="H25" s="29"/>
       <c r="I25" s="38"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5381,7 +5381,7 @@
       <c r="H26" s="29"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5407,7 +5407,7 @@
       <c r="H27" s="29"/>
       <c r="I27" s="38"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5433,7 +5433,7 @@
       <c r="H28" s="29"/>
       <c r="I28" s="38"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5459,7 +5459,7 @@
       <c r="H29" s="29"/>
       <c r="I29" s="38"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5485,7 +5485,7 @@
       <c r="H30" s="30"/>
       <c r="I30" s="39"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -5548,384 +5548,419 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="107"/>
-    <col min="2" max="2" width="39.28515625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="107" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="107"/>
-    <col min="7" max="7" width="39.42578125" style="32" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="32"/>
+    <col min="1" max="1" width="9.109375" style="104"/>
+    <col min="2" max="2" width="39.33203125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="104" customWidth="1"/>
+    <col min="4" max="6" width="9.109375" style="104"/>
+    <col min="7" max="7" width="39.44140625" style="32" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="72" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="103" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D2" s="108"/>
-    </row>
-    <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="109" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="105"/>
+    </row>
+    <row r="4" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="106" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="109" t="s">
+      <c r="D4" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="109" t="s">
+      <c r="E4" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="109" t="s">
+      <c r="F4" s="106" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="107">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="104">
         <v>1</v>
       </c>
       <c r="B5" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="107" t="s">
+      <c r="C5" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="107">
+      <c r="D5" s="104">
         <v>3</v>
       </c>
-      <c r="E5" s="107">
+      <c r="E5" s="104">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="107">
+    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="104">
         <v>2</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="107">
+      <c r="D6" s="104">
         <v>5</v>
       </c>
-      <c r="E6" s="107">
+      <c r="E6" s="104">
         <v>1</v>
       </c>
       <c r="G6" s="32" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="107">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="104">
         <v>3</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="107">
+      <c r="D7" s="104">
         <v>3</v>
       </c>
-      <c r="E7" s="107">
+      <c r="E7" s="104">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="107">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="104">
         <v>4</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="107">
+      <c r="D8" s="104">
         <v>8</v>
       </c>
-      <c r="E8" s="107">
+      <c r="E8" s="104">
         <v>3</v>
       </c>
       <c r="G8" s="98"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="107">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="104">
         <v>5</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="107" t="s">
+      <c r="C9" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="107">
+      <c r="D9" s="104">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="107">
+    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="104">
         <v>6</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="107" t="s">
+      <c r="C10" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="104">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="109" t="s">
+    <row r="11" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="106" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="109" t="s">
+      <c r="D12" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="109" t="s">
+      <c r="E12" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="109" t="s">
+      <c r="F12" s="106" t="s">
         <v>76</v>
       </c>
       <c r="G12" s="44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="107">
+    <row r="13" spans="1:7" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="104">
         <v>1</v>
       </c>
       <c r="B13" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="107" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="98" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="107">
+    <row r="14" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="104">
         <v>2</v>
       </c>
       <c r="B14" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="107">
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="104">
         <v>3</v>
       </c>
       <c r="B15" s="98" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="107">
+    <row r="16" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A16" s="104">
         <v>4</v>
       </c>
       <c r="B16" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="107" t="s">
+      <c r="C16" s="104" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="98"/>
     </row>
-    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="107">
+    <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="104">
         <v>5</v>
       </c>
       <c r="B17" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="107">
+    <row r="18" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="104">
         <v>6</v>
       </c>
       <c r="B18" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="104" t="s">
         <v>19</v>
       </c>
       <c r="G18" s="98" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="107">
+    <row r="19" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A19" s="104">
         <v>7</v>
       </c>
       <c r="B19" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="107" t="s">
+      <c r="C19" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="107">
+    <row r="20" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="104">
         <v>8</v>
       </c>
       <c r="B20" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="107" t="s">
+      <c r="C20" s="104" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="98" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="107">
+    <row r="21" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="104">
         <v>9</v>
       </c>
       <c r="B21" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="107" t="s">
+      <c r="C21" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="104" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="102">
+    <row r="22" spans="1:7" s="101" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="99">
         <v>10</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="102" t="s">
+      <c r="C22" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-    </row>
-    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="107">
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+    </row>
+    <row r="23" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="104">
         <v>11</v>
       </c>
       <c r="B23" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="107" t="s">
+      <c r="C23" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="107">
+    <row r="24" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A24" s="104">
         <v>12</v>
       </c>
       <c r="B24" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="107" t="s">
+      <c r="C24" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="107">
+    <row r="25" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="104">
         <v>13</v>
       </c>
       <c r="B25" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="107" t="s">
+      <c r="C25" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="104">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="104">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="104">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="104">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="104">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="104">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J37" s="74"/>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" s="74"/>
     </row>
-    <row r="53" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 G26:G41 A54:G163 B47:F52 A4:G11 B26:F44 A26:A52">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
       <formula>$C4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
       <formula>$C4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
       <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
       <formula>$C43="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
       <formula>$C43="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
       <formula>$C43="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:G43">
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:G25">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="1" stopIfTrue="1">
       <formula>$C12="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
       <formula>$C12="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>$C12="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5951,13 +5986,13 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1051560</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>323850</xdr:rowOff>
+                    <xdr:rowOff>327660</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5979,27 +6014,27 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="5.42578125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="6.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" hidden="1" customWidth="1"/>
-    <col min="18" max="256" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="5.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="18" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6014,7 +6049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -6032,7 +6067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>42</v>
       </c>
@@ -6044,7 +6079,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6059,7 +6094,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6070,12 +6105,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="99">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="108">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B8" s="99"/>
+      <c r="B8" s="108"/>
       <c r="D8" s="56">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
         <v>25</v>
@@ -6084,7 +6119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6103,7 +6138,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -6115,7 +6150,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -6127,7 +6162,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -6139,7 +6174,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F13" s="54" t="s">
         <v>52</v>
       </c>
@@ -6147,12 +6182,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -6161,7 +6196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -6170,7 +6205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -6186,18 +6221,18 @@
         <v>2.8284271247461903</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="99">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="108">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B18" s="99"/>
+      <c r="B18" s="108"/>
       <c r="D18" s="57">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -6213,7 +6248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -6229,7 +6264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -6238,7 +6273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -6247,7 +6282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -6256,7 +6291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -6265,25 +6300,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="101" t="s">
+    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="101"/>
-      <c r="N26" s="101"/>
-      <c r="O26" s="101" t="s">
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="110"/>
+      <c r="O26" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="P26" s="101"/>
-      <c r="Q26" s="101"/>
-    </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="110"/>
+      <c r="Q26" s="110"/>
+    </row>
+    <row r="27" spans="1:17" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="58" t="s">
         <v>13</v>
       </c>
@@ -6302,10 +6337,10 @@
       <c r="F27" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="100" t="s">
+      <c r="G27" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="100"/>
+      <c r="H27" s="109"/>
       <c r="I27" s="61" t="s">
         <v>36</v>
       </c>
@@ -6332,7 +6367,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="55">
         <v>1</v>
       </c>
@@ -6394,7 +6429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="55">
         <v>2</v>
       </c>
@@ -6457,7 +6492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="55">
         <v>3</v>
       </c>
@@ -6518,7 +6553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="55">
         <v>4</v>
       </c>
@@ -6579,7 +6614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="55">
         <v>5</v>
       </c>
@@ -6640,7 +6675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="55">
         <v>6</v>
       </c>
@@ -6699,7 +6734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="55">
         <v>7</v>
       </c>
@@ -6758,7 +6793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="55">
         <v>8</v>
       </c>
@@ -6817,7 +6852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="55">
         <v>9</v>
       </c>
@@ -6876,7 +6911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="55">
         <v>10</v>
       </c>
@@ -6935,7 +6970,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="55">
         <v>11</v>
       </c>
@@ -6994,7 +7029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="55">
         <v>12</v>
       </c>
@@ -7053,7 +7088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="55">
         <v>13</v>
       </c>
@@ -7111,7 +7146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="55">
         <v>14</v>
       </c>
@@ -7169,7 +7204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="55">
         <v>15</v>
       </c>
@@ -7227,7 +7262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="55">
         <v>16</v>
       </c>
@@ -7285,7 +7320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="55">
         <v>17</v>
       </c>
@@ -7343,7 +7378,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="55">
         <v>18</v>
       </c>
@@ -7401,7 +7436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="55">
         <v>19</v>
       </c>
@@ -7459,7 +7494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="55">
         <v>20</v>
       </c>
@@ -7517,7 +7552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="55">
         <v>21</v>
       </c>
@@ -7575,7 +7610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="55">
         <v>22</v>
       </c>
@@ -7633,7 +7668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="55">
         <v>23</v>
       </c>
@@ -7691,7 +7726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="55">
         <v>24</v>
       </c>
@@ -7759,13 +7794,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K27:N27 A27:G27 F26 I27 O26:O27 P27:Q27">
-    <cfRule type="expression" dxfId="20" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$D26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>$D26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>$D26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7787,18 +7822,18 @@
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="34" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="34" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="34" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="33" customWidth="1"/>
-    <col min="6" max="30" width="4.42578125" style="33" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="1" width="43.44140625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="33" customWidth="1"/>
+    <col min="6" max="30" width="4.44140625" style="33" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="65">
         <v>1</v>
       </c>
@@ -7830,7 +7865,7 @@
       <c r="AC1" s="34"/>
       <c r="AD1" s="34"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
@@ -7858,7 +7893,7 @@
       <c r="AC2" s="34"/>
       <c r="AD2" s="34"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="67" t="s">
         <v>12</v>
       </c>
@@ -7898,7 +7933,7 @@
       <c r="AC9" s="69"/>
       <c r="AD9" s="69"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>29</v>
       </c>
@@ -8016,7 +8051,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -8133,7 +8168,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>26</v>
       </c>
@@ -8243,7 +8278,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>27</v>
       </c>
@@ -8332,7 +8367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
         <v>7</v>
       </c>
@@ -8448,7 +8483,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -8476,7 +8511,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -8506,7 +8541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -8544,7 +8579,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -8573,7 +8608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
       <c r="C19"/>
       <c r="AC19" s="33" t="str">
@@ -8585,7 +8620,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
       <c r="C20"/>
       <c r="AC20" s="33" t="str">
@@ -8597,7 +8632,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
       <c r="C21"/>
       <c r="AC21" s="33" t="str">
@@ -8609,7 +8644,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
       <c r="C22"/>
       <c r="AC22" s="33" t="str">
@@ -8621,7 +8656,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32"/>
       <c r="C23"/>
       <c r="AC23" s="33" t="str">
@@ -8633,7 +8668,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="32"/>
       <c r="C24"/>
       <c r="AC24" s="33" t="str">
@@ -8645,11 +8680,11 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="32"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="32"/>
       <c r="C26"/>
       <c r="AC26" s="33" t="str">
@@ -8661,7 +8696,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="32"/>
       <c r="C27"/>
       <c r="AC27" s="33" t="str">
@@ -8673,7 +8708,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="32"/>
       <c r="C28"/>
       <c r="AC28" s="33" t="str">
@@ -8685,7 +8720,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
       <c r="C29"/>
       <c r="AC29" s="33" t="str">
@@ -8697,7 +8732,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
       <c r="C30"/>
       <c r="AC30" s="33" t="str">
@@ -8709,7 +8744,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
       <c r="C31"/>
       <c r="AC31" s="33" t="str">
@@ -8721,7 +8756,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
       <c r="C32"/>
       <c r="AC32" s="33" t="str">
@@ -8733,7 +8768,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="C33"/>
       <c r="AC33" s="33" t="str">
@@ -8745,7 +8780,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
       <c r="C34"/>
       <c r="AC34" s="33" t="str">
@@ -8757,11 +8792,11 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="32"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
       <c r="C36"/>
       <c r="AC36" s="33" t="str">
@@ -8773,7 +8808,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
       <c r="C37"/>
       <c r="AC37" s="33" t="str">
@@ -8785,7 +8820,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
       <c r="C38"/>
       <c r="AC38" s="33" t="str">
@@ -8797,7 +8832,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="32"/>
       <c r="C39"/>
       <c r="AC39" s="33" t="str">
@@ -8809,7 +8844,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
       <c r="C40"/>
       <c r="AC40" s="33" t="str">
@@ -8821,7 +8856,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
       <c r="C41"/>
       <c r="D41" s="34" t="str">
@@ -8841,7 +8876,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C42"/>
       <c r="D42" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8860,7 +8895,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C43"/>
       <c r="D43" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8879,7 +8914,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C44"/>
       <c r="D44" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8898,7 +8933,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C45"/>
       <c r="D45" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8917,7 +8952,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C46"/>
       <c r="D46" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8936,7 +8971,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C47"/>
       <c r="D47" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8955,7 +8990,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C48"/>
       <c r="D48" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8974,7 +9009,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49"/>
       <c r="D49" s="34" t="str">
         <f t="shared" si="6"/>
@@ -8993,7 +9028,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50"/>
       <c r="D50" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9012,7 +9047,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51"/>
       <c r="D51" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9031,7 +9066,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52"/>
       <c r="D52" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9050,7 +9085,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53"/>
       <c r="D53" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9069,7 +9104,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54"/>
       <c r="D54" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9088,7 +9123,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C55"/>
       <c r="D55" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9107,7 +9142,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56"/>
       <c r="D56" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9126,7 +9161,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57"/>
       <c r="D57" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9145,7 +9180,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C58"/>
       <c r="D58" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9164,7 +9199,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C59"/>
       <c r="D59" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9183,7 +9218,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C60"/>
       <c r="D60" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9202,7 +9237,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C61"/>
       <c r="D61" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9221,7 +9256,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C62"/>
       <c r="D62" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9328,7 +9363,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C63"/>
       <c r="D63" s="34" t="str">
         <f t="shared" si="6"/>
@@ -9435,89 +9470,89 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C64"/>
       <c r="D64" s="34" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A15:AD58">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9543,13 +9578,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>2305050</xdr:colOff>
+                    <xdr:colOff>2308860</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9565,13 +9600,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2590800</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9594,18 +9629,18 @@
       <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="2" customWidth="1"/>
-    <col min="6" max="30" width="4.42578125" style="2" customWidth="1"/>
-    <col min="31" max="256" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="2" customWidth="1"/>
+    <col min="6" max="30" width="4.44140625" style="2" customWidth="1"/>
+    <col min="31" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="31">
         <v>1</v>
       </c>
@@ -9637,7 +9672,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -9665,7 +9700,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>12</v>
       </c>
@@ -9705,7 +9740,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="21"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
@@ -9823,7 +9858,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -9939,7 +9974,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>26</v>
       </c>
@@ -10049,7 +10084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>27</v>
       </c>
@@ -10138,7 +10173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>7</v>
       </c>
@@ -10254,7 +10289,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f t="shared" ref="D15:D59" si="4">IF(A15&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10264,7 +10299,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10282,7 +10317,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10300,7 +10335,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10318,7 +10353,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10336,7 +10371,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10354,7 +10389,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10372,7 +10407,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10390,7 +10425,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10408,7 +10443,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10426,7 +10461,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10444,7 +10479,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10462,7 +10497,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10480,7 +10515,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10498,7 +10533,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10516,7 +10551,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10534,7 +10569,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D31" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10552,7 +10587,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D32" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10570,7 +10605,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D33" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10588,7 +10623,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10606,7 +10641,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D35" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10624,7 +10659,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D36" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10642,7 +10677,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10660,7 +10695,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10678,7 +10713,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10696,7 +10731,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D40" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10714,7 +10749,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D41" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10732,7 +10767,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D42" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10750,7 +10785,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D43" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10768,7 +10803,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10786,7 +10821,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D45" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10804,7 +10839,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D46" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10822,7 +10857,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10840,7 +10875,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D48" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10858,7 +10893,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10876,7 +10911,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D50" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10894,7 +10929,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D51" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10912,7 +10947,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D52" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10930,7 +10965,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D53" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10948,7 +10983,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D54" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10966,7 +11001,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D55" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10984,7 +11019,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D56" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11002,7 +11037,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D57" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11020,7 +11055,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D58" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11126,7 +11161,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D59" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11232,7 +11267,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:30" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D64" t="str">
         <f>IF(A64&lt;&gt;"","Planned","")</f>
         <v/>
@@ -11241,18 +11276,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A19:AD58 J15:AD18">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:I18">
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11278,13 +11313,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>1981200</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11300,13 +11335,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2286000</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>247650</xdr:colOff>
+                    <xdr:colOff>251460</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11328,16 +11363,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="34"/>
-    <col min="4" max="4" width="32.7109375" style="34" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="34"/>
-    <col min="6" max="6" width="32.7109375" style="34" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="3" width="9.109375" style="34"/>
+    <col min="4" max="4" width="32.6640625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="34"/>
+    <col min="6" max="6" width="32.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="s">
         <v>105</v>
       </c>
@@ -11353,7 +11388,7 @@
       <c r="E1" s="82"/>
       <c r="F1" s="83"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
         <v>107</v>
       </c>
@@ -11365,7 +11400,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="85"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="86"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -11373,7 +11408,7 @@
       <c r="E3" s="78"/>
       <c r="F3" s="87"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="88"/>
       <c r="B4" s="79"/>
       <c r="C4" s="79"/>
@@ -11381,7 +11416,7 @@
       <c r="E4" s="79"/>
       <c r="F4" s="89"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C15)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11392,7 +11427,7 @@
       <c r="E5" s="76"/>
       <c r="F5" s="95"/>
     </row>
-    <row r="6" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="90" t="s">
         <v>104</v>
       </c>
@@ -11408,8 +11443,8 @@
       </c>
       <c r="F6" s="93"/>
     </row>
-    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="80" t="s">
         <v>105</v>
       </c>
@@ -11425,7 +11460,7 @@
       <c r="E9" s="82"/>
       <c r="F9" s="83"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="84" t="s">
         <v>107</v>
       </c>
@@ -11437,7 +11472,7 @@
       <c r="E10" s="77"/>
       <c r="F10" s="85"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="86"/>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
@@ -11445,7 +11480,7 @@
       <c r="E11" s="78"/>
       <c r="F11" s="87"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="88"/>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
@@ -11453,7 +11488,7 @@
       <c r="E12" s="79"/>
       <c r="F12" s="89"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C16)</f>
         <v>Responsible Person: Tina Tester</v>
@@ -11464,7 +11499,7 @@
       <c r="E13" s="76"/>
       <c r="F13" s="95"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="90" t="s">
         <v>104</v>
       </c>
@@ -11480,8 +11515,8 @@
       </c>
       <c r="F14" s="93"/>
     </row>
-    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
         <v>105</v>
       </c>
@@ -11497,7 +11532,7 @@
       <c r="E17" s="82"/>
       <c r="F17" s="83"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="84" t="s">
         <v>107</v>
       </c>
@@ -11509,7 +11544,7 @@
       <c r="E18" s="77"/>
       <c r="F18" s="85"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="86"/>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
@@ -11517,7 +11552,7 @@
       <c r="E19" s="78"/>
       <c r="F19" s="87"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="88"/>
       <c r="B20" s="79"/>
       <c r="C20" s="79"/>
@@ -11525,7 +11560,7 @@
       <c r="E20" s="79"/>
       <c r="F20" s="89"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C17)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11536,7 +11571,7 @@
       <c r="E21" s="76"/>
       <c r="F21" s="95"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="90" t="s">
         <v>104</v>
       </c>
@@ -11552,8 +11587,8 @@
       </c>
       <c r="F22" s="93"/>
     </row>
-    <row r="24" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="80" t="s">
         <v>105</v>
       </c>
@@ -11569,7 +11604,7 @@
       <c r="E25" s="82"/>
       <c r="F25" s="83"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="84" t="s">
         <v>107</v>
       </c>
@@ -11581,7 +11616,7 @@
       <c r="E26" s="77"/>
       <c r="F26" s="85"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="86"/>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
@@ -11589,7 +11624,7 @@
       <c r="E27" s="78"/>
       <c r="F27" s="87"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="88"/>
       <c r="B28" s="79"/>
       <c r="C28" s="79"/>
@@ -11597,7 +11632,7 @@
       <c r="E28" s="79"/>
       <c r="F28" s="89"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C18)</f>
         <v xml:space="preserve">Responsible Person: </v>
@@ -11608,7 +11643,7 @@
       <c r="E29" s="76"/>
       <c r="F29" s="95"/>
     </row>
-    <row r="30" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="90" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Added 3 more user stories
References #1.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A75795-30EC-4D33-823C-B60DB8302C98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B7801-D6DF-4FCB-8CCB-38EC2444C3A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
   <si>
     <t>Goal</t>
   </si>
@@ -733,6 +733,21 @@
     <t xml:space="preserve"> - “Subscriptions” is a term we are using to loosely define service subscriptions, licenses and free trials
  - A reminder refers to an email notification from the application with details of the subscription due to expire.
  - “Close to expiring” could mean 7 days or 1 day prior to the expiration date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Number literals were chosen because they were thought to be simpler to implement than having some form of currency conversion.
+ - With the above comment in mind, this means that if a user lives in NZ and moves elsewhere, the subscription cost doesn't change. It is up to them to change the cost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. As a budgeter I want to be able to input number literals into the subscription's details so I know how much each of my clients' subscriptions cost.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. As a developer I want the system to automatically issue a reminder once the date has changed, and it is within the specified amount of days before a subscription ends. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. As a developer I want the users to have the ability to add a company that they are subscribed to when they are not able to search for it. </t>
   </si>
 </sst>
 </file>
@@ -5548,8 +5563,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="4" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5876,19 +5891,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A26" s="104">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="98" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="66" x14ac:dyDescent="0.25">
       <c r="A27" s="104">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="98" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="98"/>
+    </row>
+    <row r="28" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A28" s="104">
         <v>16</v>
+      </c>
+      <c r="B28" s="98" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a user story; updated sprint columns; added cell format options
References #1.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steam\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DFE24E0-904E-451F-A85D-1E8BFD918E40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5FF983F-47F2-49E7-AA50-089B475506B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
   <si>
     <t>Goal</t>
   </si>
@@ -739,13 +739,19 @@
     <t>As a budgeter I want to be able to input number literals into the subscription's details so I know how much each of my clients' subscriptions cost.</t>
   </si>
   <si>
-    <t>As a designer I want to be able to keep track of  the all costs of my application licenses in one place so that I can budget and price my work appropriately.</t>
-  </si>
-  <si>
     <t>As a developer I want the system to automatically issue a reminder once the date has changed, and it is within the specified amount of days before a subscription ends.</t>
   </si>
   <si>
     <t>As a developer I want the users to have the ability to add a company that they are subscribed to when they are not able to search for it.</t>
+  </si>
+  <si>
+    <t>As a user I want to update my subscription details so I can account for any unforeseen changes.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>As a designer I want to be able to keep track of all costs of my application licenses in one place so that I can budget and price my work appropriately.</t>
   </si>
 </sst>
 </file>
@@ -758,7 +764,7 @@
     <numFmt numFmtId="166" formatCode="&quot;Sprint &quot;#&quot; Backlog&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;Last &quot;###&quot; sprints&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -772,10 +778,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -832,8 +840,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -850,6 +865,41 @@
       <patternFill patternType="solid">
         <fgColor indexed="43"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF981"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor rgb="FFC00000"/>
+        <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
@@ -1230,10 +1280,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyAlignment="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyAlignment="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyAlignment="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1509,9 +1569,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1521,11 +1578,295 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Done" xfId="2" xr:uid="{3A954031-7DD0-4069-AF56-88C833BEDEA5}"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ongoing" xfId="3" xr:uid="{AA49429F-4DD8-47C8-89B0-6E0267D63520}"/>
+    <cellStyle name="Removed" xfId="4" xr:uid="{4BE2B0B7-2213-415D-B9E8-FC016EE7E552}"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="82">
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1565,14 +1906,6 @@
       <fill>
         <patternFill>
           <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1886,6 +2219,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFF981"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FF26CCB0"/>
+      <color rgb="FF9E7800"/>
+      <color rgb="FFFFCC99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4219,7 +4562,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
+      <xdr:colOff>577850</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -5070,7 +5413,7 @@
       </c>
       <c r="E4" s="22">
         <f>IF(A4="","",SUMIF(I$16:I$30,'Release Plan'!A4,E$16:E$30))</f>
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="47"/>
@@ -5251,7 +5594,7 @@
       </c>
       <c r="E16" s="22">
         <f>IF(A16="","",SUMIF('Product Backlog'!E$5:E$103,'Release Plan'!A16,'Product Backlog'!D$5:D$103))</f>
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>19</v>
@@ -5661,7 +6004,7 @@
       </c>
       <c r="E31" s="25">
         <f>SUMIF('Product Backlog'!E$6:E$103,"",'Product Backlog'!D$6:D$103)-SUMIF('Product Backlog'!C$6:C$103,"Removed",'Product Backlog'!D$6:D$103)</f>
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="F31" s="23"/>
       <c r="G31" s="50"/>
@@ -5670,29 +6013,29 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G4:H10 E31 E5:E10 A4:D10">
-    <cfRule type="expression" dxfId="48" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="1" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="2" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F10 F16:F30">
-    <cfRule type="expression" dxfId="46" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="3" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="4" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G16:H30 A16:E30">
-    <cfRule type="expression" dxfId="43" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="6" stopIfTrue="1">
       <formula>OR($F4="Planned",$F4="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="7" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5715,8 +6058,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5764,39 +6107,42 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="104">
+      <c r="A5" s="112">
         <v>1</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="104">
+      <c r="D5" s="112">
         <v>3</v>
       </c>
-      <c r="E5" s="104">
+      <c r="E5" s="112">
         <v>1</v>
       </c>
+      <c r="F5" s="112"/>
+      <c r="G5" s="114"/>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="104">
+      <c r="A6" s="110">
         <v>2</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="111" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="110" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="104">
+      <c r="D6" s="110">
         <v>5</v>
       </c>
-      <c r="E6" s="104">
+      <c r="E6" s="110">
         <v>1</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="F6" s="110"/>
+      <c r="G6" s="111" t="s">
         <v>89</v>
       </c>
     </row>
@@ -5888,35 +6234,44 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="104">
+      <c r="A13" s="115">
         <v>1</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="115" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="107" t="s">
+      <c r="C13" s="116" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="115">
+        <v>34</v>
+      </c>
+      <c r="E13" s="115">
+        <v>1</v>
+      </c>
+      <c r="F13" s="115" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="115" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="117">
+        <v>2</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="104">
-        <v>34</v>
-      </c>
-      <c r="G13" s="98" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="104">
-        <v>2</v>
-      </c>
-      <c r="B14" s="98" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="104" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="104">
+      <c r="D14" s="117">
         <v>5</v>
       </c>
+      <c r="E14" s="117"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="119"/>
     </row>
     <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="104">
@@ -6100,7 +6455,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="98" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="104" t="s">
         <v>19</v>
@@ -6114,15 +6469,18 @@
         <v>16</v>
       </c>
       <c r="B28" s="98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="104" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="104">
         <v>17</v>
+      </c>
+      <c r="B29" s="98" t="s">
+        <v>129</v>
       </c>
       <c r="C29" s="104" t="s">
         <v>19</v>
@@ -6132,6 +6490,7 @@
       <c r="A30" s="104">
         <v>18</v>
       </c>
+      <c r="B30" s="98"/>
       <c r="C30" s="104" t="s">
         <v>19</v>
       </c>
@@ -6162,124 +6521,135 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 G26:G41 A54:G163 B47:F52 A4:G11 B33:F44 A26:A52 B26:B32 D26:F32">
-    <cfRule type="expression" dxfId="41" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
       <formula>$C4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="29" stopIfTrue="1">
       <formula>$C4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="30" stopIfTrue="1">
       <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="expression" dxfId="38" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="31" stopIfTrue="1">
       <formula>$C43="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="32" stopIfTrue="1">
       <formula>$C43="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="33" stopIfTrue="1">
       <formula>$C43="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:G43">
-    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="34" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="35" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="36" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:G25">
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+  <conditionalFormatting sqref="A12:G13 A15:G25 A14 C14:G14">
+    <cfRule type="expression" dxfId="68" priority="25" stopIfTrue="1">
       <formula>$C12="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="26" stopIfTrue="1">
       <formula>$C12="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="27" stopIfTrue="1">
       <formula>$C12="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="29" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="22" stopIfTrue="1">
       <formula>$C26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="23" stopIfTrue="1">
       <formula>$C26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="24" stopIfTrue="1">
       <formula>$C26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="26" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="19" stopIfTrue="1">
       <formula>$C27="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="20" stopIfTrue="1">
       <formula>$C27="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="21" stopIfTrue="1">
       <formula>$C27="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="23" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="16" stopIfTrue="1">
       <formula>$C28="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="17" stopIfTrue="1">
       <formula>$C28="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="18" stopIfTrue="1">
       <formula>$C28="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="13" stopIfTrue="1">
       <formula>$C29="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="14" stopIfTrue="1">
       <formula>$C29="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="15" stopIfTrue="1">
       <formula>$C29="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="10" stopIfTrue="1">
       <formula>$C30="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
       <formula>$C30="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="12" stopIfTrue="1">
       <formula>$C30="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="7" stopIfTrue="1">
       <formula>$C31="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="8" stopIfTrue="1">
       <formula>$C31="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="9" stopIfTrue="1">
       <formula>$C31="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="11" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="4" stopIfTrue="1">
       <formula>$C32="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="5" stopIfTrue="1">
       <formula>$C32="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
       <formula>$C32="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>$C14="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>$C14="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>$C14="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6328,8 +6698,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6424,11 +6794,11 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="108">
+      <c r="A8" s="107">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B8" s="108"/>
+      <c r="B8" s="107"/>
       <c r="D8" s="56">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
         <v>25</v>
@@ -6540,11 +6910,11 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="108">
+      <c r="A18" s="107">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B18" s="108"/>
+      <c r="B18" s="107"/>
       <c r="D18" s="57">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
         <v>6</v>
@@ -6619,22 +6989,22 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="110" t="s">
+      <c r="F26" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="110"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="110"/>
-      <c r="L26" s="110"/>
-      <c r="M26" s="110"/>
-      <c r="N26" s="110"/>
-      <c r="O26" s="110" t="s">
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="109"/>
+      <c r="M26" s="109"/>
+      <c r="N26" s="109"/>
+      <c r="O26" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="P26" s="110"/>
-      <c r="Q26" s="110"/>
+      <c r="P26" s="109"/>
+      <c r="Q26" s="109"/>
     </row>
     <row r="27" spans="1:17" s="3" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
@@ -6655,10 +7025,10 @@
       <c r="F27" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="109" t="s">
+      <c r="G27" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="109"/>
+      <c r="H27" s="108"/>
       <c r="I27" s="61" t="s">
         <v>36</v>
       </c>
@@ -8112,13 +8482,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K27:N27 A27:G27 F26 I27 O26:O27 P27:Q27">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="1" stopIfTrue="1">
       <formula>$D26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="2" stopIfTrue="1">
       <formula>$D26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="3" stopIfTrue="1">
       <formula>$D26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9867,10 +10237,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A15:AD58">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11594,18 +11964,18 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A19:AD58 J15:AD18">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:I18">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="3" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adjusted alignment formatting for first user story
References #1.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steam\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5FF983F-47F2-49E7-AA50-089B475506B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF7D6736-A237-4CCD-B3EC-3320F2978DB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1596,9 +1596,6 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1607,6 +1604,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -6058,8 +6058,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6240,7 +6240,7 @@
       <c r="B13" s="115" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="115" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="115">
@@ -6252,26 +6252,26 @@
       <c r="F13" s="115" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="115" t="s">
+      <c r="G13" s="119" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="117">
+      <c r="A14" s="116">
         <v>2</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="117" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="117">
+      <c r="D14" s="116">
         <v>5</v>
       </c>
-      <c r="E14" s="117"/>
-      <c r="F14" s="117"/>
-      <c r="G14" s="119"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="118"/>
     </row>
     <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="104">

</xml_diff>

<commit_message>
Updated sprint-related sheets to reflect week 1 progress
References #1.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steam\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF7D6736-A237-4CCD-B3EC-3320F2978DB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB0CF2F-B514-445E-8790-B63B6E615510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
   <si>
     <t>Goal</t>
   </si>
@@ -752,6 +752,40 @@
   </si>
   <si>
     <t>As a designer I want to be able to keep track of all costs of my application licenses in one place so that I can budget and price my work appropriately.</t>
+  </si>
+  <si>
+    <t>Total Size</t>
+  </si>
+  <si>
+    <t>Total Sample Size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>See</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://isgb.otago.ac.nz/info310/syela651/SubscriptionTracker/issues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for more details</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -764,7 +798,7 @@
     <numFmt numFmtId="166" formatCode="&quot;Sprint &quot;#&quot; Backlog&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;Last &quot;###&quot; sprints&quot;"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -846,6 +880,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1280,7 +1321,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyAlignment="0">
@@ -1292,8 +1333,9 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyAlignment="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1569,15 +1611,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1596,6 +1629,9 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1605,23 +1641,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Done" xfId="2" xr:uid="{3A954031-7DD0-4069-AF56-88C833BEDEA5}"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Ongoing" xfId="3" xr:uid="{AA49429F-4DD8-47C8-89B0-6E0267D63520}"/>
     <cellStyle name="Removed" xfId="4" xr:uid="{4BE2B0B7-2213-415D-B9E8-FC016EE7E552}"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="66">
     <dxf>
       <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1710,202 +1835,6 @@
         <patternFill patternType="lightUp">
           <fgColor indexed="10"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor indexed="10"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="42"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2328,21 +2257,12 @@
               <c:f>[0]!ColTopRemainingWork</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>137</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2370,21 +2290,12 @@
               <c:f>[0]!ColTopRemainingWork</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>137</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2418,7 +2329,7 @@
               <c:f>[0]!PBCurrentBottom</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2438,6 +2349,57 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2466,21 +2428,12 @@
               <c:f>[0]!ColBottomCurrentScope</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2526,27 +2479,78 @@
               <c:f>[0]!PBTrend</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>137.66666666666669</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112.66666666666669</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.666666666666686</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.666666666666686</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.666666666666686</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.666666666666686</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2577,21 +2581,12 @@
               <c:f>[0]!ColBottomCurrentScope</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2884,21 +2879,9 @@
               <c:f>[0]!PlannedSpeed</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2932,12 +2915,9 @@
               <c:f>[0]!RealizedSpeed</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2985,21 +2965,12 @@
               <c:f>[0]!AverageSpeedRealized</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,21 +3004,12 @@
               <c:f>[0]!AverageSpeedLastEight</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3081,21 +3043,12 @@
               <c:f>[0]!AverageSpeedWorstThree</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6013,29 +5966,29 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G4:H10 E31 E5:E10 A4:D10">
-    <cfRule type="expression" dxfId="81" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="1" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="2" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F10 F16:F30">
-    <cfRule type="expression" dxfId="79" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="3" stopIfTrue="1">
       <formula>$F4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="4" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 G16:H30 A16:E30">
-    <cfRule type="expression" dxfId="76" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="6" stopIfTrue="1">
       <formula>OR($F4="Planned",$F4="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="7" stopIfTrue="1">
       <formula>$F4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6058,8 +6011,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6072,7 +6025,7 @@
     <col min="8" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="72" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="72" x14ac:dyDescent="0.2">
       <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
@@ -6080,10 +6033,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D2" s="105"/>
     </row>
-    <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="106" t="s">
         <v>21</v>
       </c>
@@ -6106,47 +6059,50 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="112">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="109">
         <v>1</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="112">
+      <c r="D5" s="109">
         <v>3</v>
       </c>
-      <c r="E5" s="112">
+      <c r="E5" s="109">
         <v>1</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="114"/>
-    </row>
-    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="110">
+      <c r="F5" s="109"/>
+      <c r="G5" s="111"/>
+    </row>
+    <row r="6" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="107">
         <v>2</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="110">
+      <c r="D6" s="107">
         <v>5</v>
       </c>
-      <c r="E6" s="110">
+      <c r="E6" s="107">
         <v>1</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="111" t="s">
+      <c r="F6" s="107"/>
+      <c r="G6" s="108" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J6" s="44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="104">
         <v>3</v>
       </c>
@@ -6162,8 +6118,12 @@
       <c r="E7" s="104">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J7" s="32">
+        <f>SUM(D5:D10)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="104">
         <v>4</v>
       </c>
@@ -6181,7 +6141,7 @@
       </c>
       <c r="G8" s="98"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="104">
         <v>5</v>
       </c>
@@ -6195,7 +6155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="104">
         <v>6</v>
       </c>
@@ -6209,8 +6169,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="106" t="s">
         <v>21</v>
       </c>
@@ -6232,48 +6192,55 @@
       <c r="G12" s="44" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="115">
+      <c r="J12" s="44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="112">
         <v>1</v>
       </c>
-      <c r="B13" s="115" t="s">
+      <c r="B13" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="115">
+      <c r="D13" s="112">
         <v>34</v>
       </c>
-      <c r="E13" s="115">
+      <c r="E13" s="112">
         <v>1</v>
       </c>
-      <c r="F13" s="115" t="s">
+      <c r="F13" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="119" t="s">
+      <c r="G13" s="120" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="116">
+      <c r="J13" s="32">
+        <f>SUM(D:D)-J7</f>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="114">
         <v>2</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="115" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="116">
+      <c r="D14" s="114">
         <v>5</v>
       </c>
-      <c r="E14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="118"/>
-    </row>
-    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E14" s="114"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="116"/>
+    </row>
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="104">
         <v>3</v>
       </c>
@@ -6287,7 +6254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="104">
         <v>4</v>
       </c>
@@ -6521,135 +6488,157 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 G26:G41 A54:G163 B47:F52 A4:G11 B33:F44 A26:A52 B26:B32 D26:F32">
-    <cfRule type="expression" dxfId="8" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="34" stopIfTrue="1">
       <formula>$C4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="35" stopIfTrue="1">
       <formula>$C4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="36" stopIfTrue="1">
       <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53">
-    <cfRule type="expression" dxfId="74" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="37" stopIfTrue="1">
       <formula>$C43="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="38" stopIfTrue="1">
       <formula>$C43="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="39" stopIfTrue="1">
       <formula>$C43="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:G43">
-    <cfRule type="expression" dxfId="71" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="40" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="41" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="42" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:G13 A15:G25 A14 C14:G14">
-    <cfRule type="expression" dxfId="68" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="31" stopIfTrue="1">
       <formula>$C12="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="32" stopIfTrue="1">
       <formula>$C12="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="33" stopIfTrue="1">
       <formula>$C12="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="65" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="28" stopIfTrue="1">
       <formula>$C26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="29" stopIfTrue="1">
       <formula>$C26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="30" stopIfTrue="1">
       <formula>$C26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="62" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="25" stopIfTrue="1">
       <formula>$C27="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="26" stopIfTrue="1">
       <formula>$C27="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="27" stopIfTrue="1">
       <formula>$C27="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="59" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="22" stopIfTrue="1">
       <formula>$C28="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="23" stopIfTrue="1">
       <formula>$C28="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="24" stopIfTrue="1">
       <formula>$C28="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="56" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="19" stopIfTrue="1">
       <formula>$C29="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="20" stopIfTrue="1">
       <formula>$C29="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="21" stopIfTrue="1">
       <formula>$C29="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="53" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="16" stopIfTrue="1">
       <formula>$C30="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="17" stopIfTrue="1">
       <formula>$C30="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="18" stopIfTrue="1">
       <formula>$C30="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="50" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
       <formula>$C31="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
       <formula>$C31="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="15" stopIfTrue="1">
       <formula>$C31="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="47" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>$C32="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
       <formula>$C32="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
       <formula>$C32="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="7" stopIfTrue="1">
       <formula>$C14="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="8" stopIfTrue="1">
       <formula>$C14="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
       <formula>$C14="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="expression" dxfId="22" priority="4" stopIfTrue="1">
+      <formula>$C12="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+      <formula>$C12="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+      <formula>$C12="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6">
+    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
+      <formula>$C4="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="2" stopIfTrue="1">
+      <formula>$C4="Ongoing"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+      <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6699,13 +6688,14 @@
   <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="4" width="8.7109375" customWidth="1"/>
+    <col min="2" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="5.42578125" hidden="1" customWidth="1"/>
@@ -6727,14 +6717,14 @@
         <v>37</v>
       </c>
       <c r="D3">
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="53">
         <f>IF(COUNT(B28:B39)=0,1,COUNT(B28:B39))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -6752,7 +6742,7 @@
       </c>
       <c r="G4" s="53">
         <f>IF(COUNT(D28:D51)=0,1,COUNT(D28:D51)+1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -6776,7 +6766,7 @@
       </c>
       <c r="G6" s="53">
         <f>TrendSprintCount-TrendOffset</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Z6" s="37" t="s">
         <v>96</v>
@@ -6794,14 +6784,14 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="107">
+      <c r="A8" s="117">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B8" s="107"/>
+      <c r="B8" s="117"/>
       <c r="D8" s="56">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Z8" s="37" t="s">
         <v>100</v>
@@ -6813,14 +6803,14 @@
       </c>
       <c r="D9" s="56">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,1,0,SprintCount,1)))</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
       </c>
       <c r="G9" s="53">
         <f ca="1">IF(M28="",1,COUNT(M28:M110))</f>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="Z9" s="37" t="s">
         <v>101</v>
@@ -6832,7 +6822,7 @@
       </c>
       <c r="D10" s="56">
         <f ca="1">IF(D28="","",AVERAGE(LastEight))</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Z10" s="37" t="s">
         <v>97</v>
@@ -6844,7 +6834,7 @@
       </c>
       <c r="D11" s="56">
         <f ca="1">IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(LastEight,1),SMALL(LastEight,2),SMALL(LastEight,3))))</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="37" t="s">
         <v>98</v>
@@ -6856,7 +6846,7 @@
       </c>
       <c r="D12" s="56">
         <f ca="1">IF(M29="","",M28-M29)</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Z12" s="37" t="s">
         <v>102</v>
@@ -6881,7 +6871,7 @@
       </c>
       <c r="D15" s="57">
         <f>IF(D7="",0,ROUNDUP(D3/D7*0.6,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -6890,7 +6880,7 @@
       </c>
       <c r="D16" s="57">
         <f>IF(D7="",0,ROUNDUP(D3/D7,0))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -6899,25 +6889,25 @@
       </c>
       <c r="D17" s="57">
         <f>IF(D7="",0,ROUNDUP(D3/D7*1.6,0))</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
       </c>
       <c r="G17">
         <f>IF(OR(D28="",D29=""),1,STDEV(D28:D51))</f>
-        <v>2.8284271247461903</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="107">
+      <c r="A18" s="117">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B18" s="107"/>
+      <c r="B18" s="117"/>
       <c r="D18" s="57">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -6926,14 +6916,14 @@
       </c>
       <c r="D19" s="57">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/D9+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D9,0)+SprintCount))</f>
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
         <v>63</v>
       </c>
       <c r="G19">
         <f ca="1">LastPlanned</f>
-        <v>28</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -6942,7 +6932,7 @@
       </c>
       <c r="D20" s="57">
         <f ca="1">IF(D10="","",IF(LastRealized="",ROUNDUP(LastPlanned/D10+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D10,0)+SprintCount))</f>
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -6958,7 +6948,7 @@
       </c>
       <c r="D21" s="57">
         <f ca="1">IF(D11="","",IF(LastRealized="",ROUNDUP(LastPlanned/D11+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D11,0)+SprintCount))</f>
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -6967,7 +6957,7 @@
       </c>
       <c r="D22" s="57">
         <f ca="1">IF(COUNT(M28:M51)-1&gt;0,COUNT(M28:M51)-1,"")</f>
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -6976,7 +6966,7 @@
       </c>
       <c r="D23" s="57">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9+G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9+G17)+SprintCount,0)))</f>
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -6985,26 +6975,26 @@
       </c>
       <c r="D24" s="57">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9-G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9-G17)+SprintCount,0)))</f>
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="109" t="s">
+      <c r="F26" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
-      <c r="O26" s="109" t="s">
+      <c r="G26" s="119"/>
+      <c r="H26" s="119"/>
+      <c r="I26" s="119"/>
+      <c r="J26" s="119"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="119"/>
+      <c r="M26" s="119"/>
+      <c r="N26" s="119"/>
+      <c r="O26" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="P26" s="109"/>
-      <c r="Q26" s="109"/>
+      <c r="P26" s="119"/>
+      <c r="Q26" s="119"/>
     </row>
     <row r="27" spans="1:17" s="3" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
@@ -7025,10 +7015,10 @@
       <c r="F27" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="108" t="s">
+      <c r="G27" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="108"/>
+      <c r="H27" s="118"/>
       <c r="I27" s="61" t="s">
         <v>36</v>
       </c>
@@ -7061,25 +7051,25 @@
       </c>
       <c r="B28" s="2">
         <f>D3</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E28" s="55">
         <f>B28</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="F28" s="53">
         <f>B28</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="G28" s="53">
         <f t="shared" ref="G28:G51" si="0">F28</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="H28" s="53">
         <f t="shared" ref="H28:H33" si="1">I28</f>
@@ -7090,15 +7080,15 @@
       </c>
       <c r="K28">
         <f t="shared" ref="K28:K33" si="2">IF(F28&lt;I28,I28,F28)</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="L28" s="53">
         <f t="shared" ref="L28:L51" ca="1" si="3">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28)&lt;N28,N28,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28))</f>
-        <v>137.66666666666669</v>
+        <v>237</v>
       </c>
       <c r="M28" s="53">
         <f ca="1">L28</f>
-        <v>137.66666666666669</v>
+        <v>237</v>
       </c>
       <c r="N28" s="53">
         <f t="shared" ref="N28:N51" ca="1" si="4">OFFSET($I$27,TrendSprintCount,0,1,1)</f>
@@ -7106,15 +7096,15 @@
       </c>
       <c r="O28" s="64">
         <f t="shared" ref="O28:O51" ca="1" si="5">D$9</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P28" s="64">
         <f t="shared" ref="P28:P51" ca="1" si="6">D$10</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q28" s="64">
         <f t="shared" ref="Q28:Q51" ca="1" si="7">D$11</f>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -7123,25 +7113,21 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" ref="B29:B51" si="8">IF(OR(B28="",C28=""),"",IF(D28="",IF(B28-C28&lt;=0,"",B28-C28),IF(B28-D28&lt;=0,"",B28-D28)))</f>
-        <v>114</v>
-      </c>
-      <c r="C29" s="2">
-        <v>29</v>
-      </c>
-      <c r="D29" s="2">
-        <v>27</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="55">
         <f>IF(B29="","",IF(D28="",E28,B29+SUM(D$28:D28)))</f>
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="F29" s="53">
         <f t="shared" ref="F29:F34" si="9">IF(B29="",IF(B28="","",IF(D28="","",I28)),IF(AND(D28="",C28=""),"",IF(AND(D28="",C28&lt;&gt;""),IF(I28&gt;F28,F28,I28),F28-D28)))</f>
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="G29" s="53">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="H29" s="53">
         <f t="shared" si="1"/>
@@ -7153,15 +7139,15 @@
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="L29" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>112.66666666666669</v>
+        <v>233</v>
       </c>
       <c r="M29" s="53">
         <f ca="1">IF(L29=L28,"",L29)</f>
-        <v>112.66666666666669</v>
+        <v>233</v>
       </c>
       <c r="N29" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7169,60 +7155,58 @@
       </c>
       <c r="O29" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P29" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q29" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="55">
         <v>3</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>87</v>
-      </c>
-      <c r="C30" s="2">
-        <v>31</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="55">
+      <c r="E30" s="55" t="str">
         <f>IF(B30="","",IF(D29="",E29,B30+SUM(D$28:D29)))</f>
-        <v>137</v>
-      </c>
-      <c r="F30" s="53">
+        <v/>
+      </c>
+      <c r="F30" s="53" t="str">
         <f t="shared" si="9"/>
-        <v>87</v>
-      </c>
-      <c r="G30" s="53">
+        <v/>
+      </c>
+      <c r="G30" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="H30" s="53">
+        <v/>
+      </c>
+      <c r="H30" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="53">
+        <v/>
+      </c>
+      <c r="I30" s="53" t="str">
         <f>IF(B30="",IF(B29="","",IF(D29="","",F29-D29)),IF(AND(C29="",D29=""),"",IF(AND(D29="",C29&lt;&gt;""),IF(I29&gt;F29,I29-C29,F29-C29),B$28-B30-SUM(D$28:D29))))</f>
-        <v>0</v>
-      </c>
-      <c r="K30">
+        <v/>
+      </c>
+      <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v/>
       </c>
       <c r="L30" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>87.666666666666686</v>
+        <v>229</v>
       </c>
       <c r="M30" s="53">
         <f t="shared" ref="M30:M51" ca="1" si="10">IF(L30=L29,"",L30)</f>
-        <v>87.666666666666686</v>
+        <v>229</v>
       </c>
       <c r="N30" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7230,60 +7214,58 @@
       </c>
       <c r="O30" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P30" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q30" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="55">
         <v>4</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>56</v>
-      </c>
-      <c r="C31" s="2">
-        <v>28</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="55">
+      <c r="E31" s="55" t="str">
         <f>IF(B31="","",IF(D30="",E30,B31+SUM(D$28:D30)))</f>
-        <v>137</v>
-      </c>
-      <c r="F31" s="53">
+        <v/>
+      </c>
+      <c r="F31" s="53" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="53">
+        <v/>
+      </c>
+      <c r="G31" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="53">
+        <v/>
+      </c>
+      <c r="H31" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="I31" s="53">
+        <v/>
+      </c>
+      <c r="I31" s="53" t="str">
         <f>IF(B31="",IF(B30="","",IF(D30="","",F30-D30)),IF(AND(C30="",D30=""),"",IF(AND(D30="",C30&lt;&gt;""),IF(I30&gt;F30,I30-C30,F30-C30),B$28-B31-SUM(D$28:D30))))</f>
-        <v>56</v>
-      </c>
-      <c r="K31">
+        <v/>
+      </c>
+      <c r="K31" t="str">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v/>
       </c>
       <c r="L31" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>62.666666666666686</v>
+        <v>225</v>
       </c>
       <c r="M31" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v>62.666666666666686</v>
+        <v>225</v>
       </c>
       <c r="N31" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7291,60 +7273,58 @@
       </c>
       <c r="O31" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P31" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q31" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="55">
         <v>5</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="2" t="str">
         <f>IF(OR(B31="",C31=""),"",IF(D31="",IF(B31-C31&lt;=0,"",B31-C31),IF(B31-D31&lt;=0,"",B31-D31)))</f>
-        <v>28</v>
-      </c>
-      <c r="C32" s="2">
-        <v>28</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="55">
+      <c r="E32" s="55" t="str">
         <f>IF(B32="","",IF(D31="",E31,B32+SUM(D$28:D31)))</f>
-        <v>137</v>
-      </c>
-      <c r="F32" s="53">
+        <v/>
+      </c>
+      <c r="F32" s="53" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="53">
+        <v/>
+      </c>
+      <c r="G32" s="53" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="53">
+        <v/>
+      </c>
+      <c r="H32" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="I32" s="53">
+        <v/>
+      </c>
+      <c r="I32" s="53" t="str">
         <f>IF(B32="",IF(B31="","",IF(D31="","",F31-D31)),IF(AND(C31="",D31=""),"",IF(AND(D31="",C31&lt;&gt;""),IF(I31&gt;F31,I31-C31,F31-C31),B$28-B32-SUM(D$28:D31))))</f>
-        <v>28</v>
-      </c>
-      <c r="K32">
+        <v/>
+      </c>
+      <c r="K32" t="str">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v/>
       </c>
       <c r="L32" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>37.666666666666686</v>
+        <v>221</v>
       </c>
       <c r="M32" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v>37.666666666666686</v>
+        <v>221</v>
       </c>
       <c r="N32" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7352,15 +7332,15 @@
       </c>
       <c r="O32" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P32" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q32" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -7399,11 +7379,11 @@
       </c>
       <c r="L33" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>12.666666666666686</v>
+        <v>217</v>
       </c>
       <c r="M33" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v>12.666666666666686</v>
+        <v>217</v>
       </c>
       <c r="N33" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7411,15 +7391,15 @@
       </c>
       <c r="O33" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P33" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q33" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -7458,11 +7438,11 @@
       </c>
       <c r="L34" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="M34" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="N34" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7470,15 +7450,15 @@
       </c>
       <c r="O34" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P34" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q34" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -7517,11 +7497,11 @@
       </c>
       <c r="L35" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M35" s="53" t="str">
+        <v>209</v>
+      </c>
+      <c r="M35" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>209</v>
       </c>
       <c r="N35" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7529,15 +7509,15 @@
       </c>
       <c r="O35" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P35" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q35" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -7576,11 +7556,11 @@
       </c>
       <c r="L36" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="53" t="str">
+        <v>205</v>
+      </c>
+      <c r="M36" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>205</v>
       </c>
       <c r="N36" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7588,15 +7568,15 @@
       </c>
       <c r="O36" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P36" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q36" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -7635,11 +7615,11 @@
       </c>
       <c r="L37" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="53" t="str">
+        <v>201</v>
+      </c>
+      <c r="M37" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>201</v>
       </c>
       <c r="N37" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7647,15 +7627,15 @@
       </c>
       <c r="O37" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P37" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q37" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -7694,11 +7674,11 @@
       </c>
       <c r="L38" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M38" s="53" t="str">
+        <v>197</v>
+      </c>
+      <c r="M38" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>197</v>
       </c>
       <c r="N38" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7706,15 +7686,15 @@
       </c>
       <c r="O38" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P38" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q38" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -7753,11 +7733,11 @@
       </c>
       <c r="L39" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="53" t="str">
+        <v>193</v>
+      </c>
+      <c r="M39" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>193</v>
       </c>
       <c r="N39" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7765,15 +7745,15 @@
       </c>
       <c r="O39" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P39" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q39" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -7811,11 +7791,11 @@
       </c>
       <c r="L40" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M40" s="53" t="str">
+        <v>189</v>
+      </c>
+      <c r="M40" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>189</v>
       </c>
       <c r="N40" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7823,15 +7803,15 @@
       </c>
       <c r="O40" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P40" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q40" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
@@ -7869,11 +7849,11 @@
       </c>
       <c r="L41" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="53" t="str">
+        <v>185</v>
+      </c>
+      <c r="M41" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>185</v>
       </c>
       <c r="N41" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7881,15 +7861,15 @@
       </c>
       <c r="O41" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P41" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q41" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -7927,11 +7907,11 @@
       </c>
       <c r="L42" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="53" t="str">
+        <v>181</v>
+      </c>
+      <c r="M42" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>181</v>
       </c>
       <c r="N42" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7939,15 +7919,15 @@
       </c>
       <c r="O42" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P42" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q42" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -7985,11 +7965,11 @@
       </c>
       <c r="L43" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="53" t="str">
+        <v>177</v>
+      </c>
+      <c r="M43" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>177</v>
       </c>
       <c r="N43" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -7997,15 +7977,15 @@
       </c>
       <c r="O43" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P43" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q43" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -8043,11 +8023,11 @@
       </c>
       <c r="L44" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="53" t="str">
+        <v>173</v>
+      </c>
+      <c r="M44" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>173</v>
       </c>
       <c r="N44" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8055,15 +8035,15 @@
       </c>
       <c r="O44" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P44" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q44" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -8101,11 +8081,11 @@
       </c>
       <c r="L45" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="53" t="str">
+        <v>169</v>
+      </c>
+      <c r="M45" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>169</v>
       </c>
       <c r="N45" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8113,15 +8093,15 @@
       </c>
       <c r="O45" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P45" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q45" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -8159,11 +8139,11 @@
       </c>
       <c r="L46" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="53" t="str">
+        <v>165</v>
+      </c>
+      <c r="M46" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>165</v>
       </c>
       <c r="N46" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8171,15 +8151,15 @@
       </c>
       <c r="O46" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P46" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q46" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -8217,11 +8197,11 @@
       </c>
       <c r="L47" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="53" t="str">
+        <v>161</v>
+      </c>
+      <c r="M47" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>161</v>
       </c>
       <c r="N47" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8229,15 +8209,15 @@
       </c>
       <c r="O47" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P47" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q47" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -8275,11 +8255,11 @@
       </c>
       <c r="L48" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="53" t="str">
+        <v>157</v>
+      </c>
+      <c r="M48" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>157</v>
       </c>
       <c r="N48" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8287,15 +8267,15 @@
       </c>
       <c r="O48" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P48" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q48" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -8333,11 +8313,11 @@
       </c>
       <c r="L49" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M49" s="53" t="str">
+        <v>153</v>
+      </c>
+      <c r="M49" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>153</v>
       </c>
       <c r="N49" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8345,15 +8325,15 @@
       </c>
       <c r="O49" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P49" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q49" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
@@ -8391,11 +8371,11 @@
       </c>
       <c r="L50" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M50" s="53" t="str">
+        <v>149</v>
+      </c>
+      <c r="M50" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>149</v>
       </c>
       <c r="N50" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8403,15 +8383,15 @@
       </c>
       <c r="O50" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P50" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q50" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
@@ -8449,11 +8429,11 @@
       </c>
       <c r="L51" s="53">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="53" t="str">
+        <v>145</v>
+      </c>
+      <c r="M51" s="53">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>145</v>
       </c>
       <c r="N51" s="53">
         <f t="shared" ca="1" si="4"/>
@@ -8461,15 +8441,15 @@
       </c>
       <c r="O51" s="64">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P51" s="64">
         <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q51" s="64">
         <f t="shared" ca="1" si="7"/>
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -8482,13 +8462,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K27:N27 A27:G27 F26 I27 O26:O27 P27:Q27">
-    <cfRule type="expression" dxfId="44" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
       <formula>$D26="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$D26="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$D26="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8503,11 +8483,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:AD87"/>
+  <dimension ref="A1:AF87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8518,10 +8498,12 @@
     <col min="4" max="4" width="10.7109375" style="34" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="33" customWidth="1"/>
     <col min="6" max="30" width="4.42578125" style="33" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="34"/>
+    <col min="31" max="31" width="9.140625" style="34"/>
+    <col min="32" max="32" width="41.140625" style="34" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="65">
         <v>1</v>
       </c>
@@ -8553,7 +8535,7 @@
       <c r="AC1" s="34"/>
       <c r="AD1" s="34"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
@@ -8581,7 +8563,7 @@
       <c r="AC2" s="34"/>
       <c r="AD2" s="34"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="67" t="s">
         <v>12</v>
       </c>
@@ -8621,7 +8603,7 @@
       <c r="AC9" s="69"/>
       <c r="AD9" s="69"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="67" t="s">
         <v>29</v>
       </c>
@@ -8739,7 +8721,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -8856,7 +8838,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>26</v>
       </c>
@@ -8966,7 +8948,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>27</v>
       </c>
@@ -9055,7 +9037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="67" t="s">
         <v>7</v>
       </c>
@@ -9171,7 +9153,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -9198,8 +9180,11 @@
         <v>0</v>
       </c>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AF15" s="121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -9309,7 +9294,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
+      <c r="B20"/>
       <c r="C20"/>
       <c r="AC20" s="33" t="str">
         <f t="shared" si="4"/>
@@ -10236,12 +10221,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A15:AD58">
-    <cfRule type="expression" dxfId="41" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A15:AD19 A21:AD58 B20:AD20">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF15">
+    <cfRule type="expression" dxfId="11" priority="45" stopIfTrue="1">
+      <formula>$D20="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="46" stopIfTrue="1">
+      <formula>$D20="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -10310,11 +10303,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AD64"/>
+  <dimension ref="A1:AF64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomLeft" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10325,10 +10318,12 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="2" customWidth="1"/>
     <col min="6" max="30" width="4.42578125" style="2" customWidth="1"/>
-    <col min="31" max="256" width="8.7109375" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" customWidth="1"/>
+    <col min="32" max="32" width="45.140625" customWidth="1"/>
+    <col min="33" max="256" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="31">
         <v>1</v>
       </c>
@@ -10360,7 +10355,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -10388,7 +10383,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>12</v>
       </c>
@@ -10428,7 +10423,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="21"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
@@ -10546,7 +10541,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -10662,7 +10657,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>26</v>
       </c>
@@ -10772,7 +10767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="s">
         <v>27</v>
       </c>
@@ -10861,7 +10856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>7</v>
       </c>
@@ -10977,7 +10972,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="38.25" x14ac:dyDescent="0.2">
       <c r="D15" t="str">
         <f t="shared" ref="D15:D59" si="4">IF(A15&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10986,8 +10981,11 @@
         <f t="shared" ref="F15:F59" si="5">IF(OR(F$14="",$E15=""),"",E15)</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AF15" s="121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11097,7 +11095,7 @@
     </row>
     <row r="22" spans="4:30" x14ac:dyDescent="0.2">
       <c r="D22" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A22&lt;&gt;"","Planned","")</f>
         <v/>
       </c>
       <c r="F22" s="2" t="str">
@@ -11963,20 +11961,28 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A19:AD58 J15:AD18">
-    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A19:AD21 J15:AD18 A23:AD58 B22:AD22">
+    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:I18">
-    <cfRule type="expression" dxfId="37" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>$D15="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>$D15="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF15">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>$D22="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+      <formula>$D22="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -12047,9 +12053,11 @@
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12057,10 +12065,12 @@
     <col min="4" max="4" width="32.7109375" style="34" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="34"/>
     <col min="6" max="6" width="32.7109375" style="34" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="34"/>
+    <col min="7" max="7" width="9.140625" style="34"/>
+    <col min="8" max="8" width="41.7109375" style="34" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="80" t="s">
         <v>105</v>
       </c>
@@ -12076,7 +12086,7 @@
       <c r="E1" s="82"/>
       <c r="F1" s="83"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>107</v>
       </c>
@@ -12087,8 +12097,11 @@
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
       <c r="F2" s="85"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" s="121" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="86"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -12096,7 +12109,7 @@
       <c r="E3" s="78"/>
       <c r="F3" s="87"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="88"/>
       <c r="B4" s="79"/>
       <c r="C4" s="79"/>
@@ -12104,7 +12117,7 @@
       <c r="E4" s="79"/>
       <c r="F4" s="89"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C15)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -12115,7 +12128,7 @@
       <c r="E5" s="76"/>
       <c r="F5" s="95"/>
     </row>
-    <row r="6" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="90" t="s">
         <v>104</v>
       </c>
@@ -12131,8 +12144,8 @@
       </c>
       <c r="F6" s="93"/>
     </row>
-    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="80" t="s">
         <v>105</v>
       </c>
@@ -12148,7 +12161,7 @@
       <c r="E9" s="82"/>
       <c r="F9" s="83"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="84" t="s">
         <v>107</v>
       </c>
@@ -12160,7 +12173,7 @@
       <c r="E10" s="77"/>
       <c r="F10" s="85"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="86"/>
       <c r="B11" s="78"/>
       <c r="C11" s="78"/>
@@ -12168,7 +12181,7 @@
       <c r="E11" s="78"/>
       <c r="F11" s="87"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="88"/>
       <c r="B12" s="79"/>
       <c r="C12" s="79"/>
@@ -12176,7 +12189,7 @@
       <c r="E12" s="79"/>
       <c r="F12" s="89"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="94" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C16)</f>
         <v>Responsible Person: Tina Tester</v>
@@ -12187,7 +12200,7 @@
       <c r="E13" s="76"/>
       <c r="F13" s="95"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>104</v>
       </c>
@@ -12203,7 +12216,7 @@
       </c>
       <c r="F14" s="93"/>
     </row>
-    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="80" t="s">
         <v>105</v>
@@ -12349,6 +12362,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>$D9="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>$D9="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" fitToHeight="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Enlarged heights for some cells
References #1.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steam\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C2AAB-6FB8-487A-8EDC-DA938DDD8FE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765E326F-3718-4F48-B5C0-C88E666491D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="7" r:id="rId1"/>
@@ -4985,7 +4985,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -5619,9 +5619,9 @@
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5780,7 +5780,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="103">
         <v>6</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="103">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
updated burndown chart and user stories
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeah2\Documents\NetBeansProjects\INFO310\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmabrothers/Documents/SubscriptionTracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF33805-A44E-4ECB-BDAE-50A709A49AAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AD9F59-0E2E-4746-BDC1-D580375D2052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="522" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="32580" windowHeight="20200" tabRatio="522" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="7" r:id="rId1"/>
@@ -1240,7 +1240,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1555,6 +1555,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Done" xfId="2" xr:uid="{3A954031-7DD0-4069-AF56-88C833BEDEA5}"/>
@@ -1837,7 +1840,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1927,7 +1930,7 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1963,7 +1966,7 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2047,7 +2050,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>158</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2098,13 +2101,13 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>213.99999999999997</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>167.99999999999997</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2143,7 +2146,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>158</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2346,7 +2349,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2480,7 +2483,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2530,13 +2533,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2572,13 +2575,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2614,13 +2617,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2837,7 +2840,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3411,7 +3414,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4011,13 +4014,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>1057275</xdr:colOff>
+          <xdr:colOff>1054100</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>333375</xdr:rowOff>
+          <xdr:rowOff>330200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4049,19 +4052,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-ZW" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
+                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Sort Product Backlog</a:t>
               </a:r>
@@ -4204,13 +4207,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2314575</xdr:colOff>
+          <xdr:colOff>2311400</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4242,19 +4245,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-ZW" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
+                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Sort Sprint Tasks</a:t>
               </a:r>
@@ -4273,13 +4276,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2590800</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4311,19 +4314,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-ZW" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
+                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Update Task Slips</a:t>
               </a:r>
@@ -4385,13 +4388,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>1981200</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4423,19 +4426,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-ZW" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
+                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Sort Sprint Tasks</a:t>
               </a:r>
@@ -4454,13 +4457,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2286000</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>104775</xdr:rowOff>
+          <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>254000</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4492,19 +4495,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-ZW" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
+                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Update Task Slips</a:t>
               </a:r>
@@ -4874,25 +4877,25 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.73046875" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" customWidth="1"/>
-    <col min="4" max="5" width="10.73046875" customWidth="1"/>
-    <col min="6" max="6" width="8.73046875" customWidth="1"/>
-    <col min="7" max="7" width="13.73046875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="59.1328125" customWidth="1"/>
-    <col min="9" max="9" width="10.73046875" customWidth="1"/>
-    <col min="10" max="256" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="59.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
@@ -4920,7 +4923,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -4944,7 +4947,7 @@
       <c r="G4" s="46"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>2</v>
       </c>
@@ -4968,7 +4971,7 @@
       <c r="G5" s="47"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="13"/>
       <c r="B6" s="39"/>
       <c r="C6" s="22" t="str">
@@ -4987,7 +4990,7 @@
       <c r="G6" s="47"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="13"/>
       <c r="B7" s="39"/>
       <c r="C7" s="22" t="str">
@@ -5006,7 +5009,7 @@
       <c r="G7" s="47"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="39"/>
       <c r="C8" s="22" t="str">
@@ -5025,7 +5028,7 @@
       <c r="G8" s="47"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="39"/>
       <c r="C9" s="22" t="str">
@@ -5044,7 +5047,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="14"/>
       <c r="B10" s="40"/>
       <c r="C10" s="41" t="str">
@@ -5063,17 +5066,17 @@
       <c r="G10" s="48"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -5103,7 +5106,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="22">
         <v>1</v>
       </c>
@@ -5131,7 +5134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="22">
         <v>2</v>
       </c>
@@ -5160,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="22">
         <v>3</v>
       </c>
@@ -5190,7 +5193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="22"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
@@ -5201,7 +5204,7 @@
       <c r="H19" s="28"/>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="22"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
@@ -5212,7 +5215,7 @@
       <c r="H20" s="28"/>
       <c r="I20" s="37"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="22"/>
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
@@ -5223,7 +5226,7 @@
       <c r="H21" s="28"/>
       <c r="I21" s="37"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="22"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
@@ -5234,7 +5237,7 @@
       <c r="H22" s="28"/>
       <c r="I22" s="37"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="str">
         <f t="shared" ref="A23:A30" si="3">IF(AND(B23&lt;&gt;"",C23&lt;&gt;""),A22+1,"")</f>
         <v/>
@@ -5260,7 +5263,7 @@
       <c r="H23" s="28"/>
       <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5286,7 +5289,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="37"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5312,7 +5315,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5338,7 +5341,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="37"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5364,7 +5367,7 @@
       <c r="H27" s="28"/>
       <c r="I27" s="37"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5390,7 +5393,7 @@
       <c r="H28" s="28"/>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5416,7 +5419,7 @@
       <c r="H29" s="28"/>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5442,7 +5445,7 @@
       <c r="H30" s="29"/>
       <c r="I30" s="38"/>
     </row>
-    <row r="31" spans="1:9" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -5506,20 +5509,20 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="103"/>
-    <col min="2" max="2" width="39.265625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" style="103" customWidth="1"/>
-    <col min="4" max="6" width="9.1328125" style="103"/>
-    <col min="7" max="7" width="39.3984375" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="31"/>
+    <col min="1" max="1" width="9.1640625" style="103"/>
+    <col min="2" max="2" width="39.33203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="103" customWidth="1"/>
+    <col min="4" max="6" width="9.1640625" style="103"/>
+    <col min="7" max="7" width="39.33203125" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="76" x14ac:dyDescent="0.15">
       <c r="A1" s="101" t="s">
         <v>5</v>
       </c>
@@ -5527,10 +5530,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D2" s="104"/>
     </row>
-    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="105" t="s">
         <v>21</v>
       </c>
@@ -5553,7 +5556,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="102.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="113" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="106">
         <v>1</v>
       </c>
@@ -5561,7 +5564,7 @@
         <v>100</v>
       </c>
       <c r="C5" s="107" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="106">
         <v>34</v>
@@ -5579,7 +5582,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A6" s="108">
         <v>2</v>
       </c>
@@ -5587,7 +5590,7 @@
         <v>120</v>
       </c>
       <c r="C6" s="108" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D6" s="108">
         <v>5</v>
@@ -5604,7 +5607,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="103">
         <v>3</v>
       </c>
@@ -5612,7 +5615,7 @@
         <v>101</v>
       </c>
       <c r="C7" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D7" s="103">
         <v>13</v>
@@ -5624,7 +5627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="63.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.15">
       <c r="A8" s="103">
         <v>4</v>
       </c>
@@ -5632,7 +5635,7 @@
         <v>102</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" s="103">
         <v>2</v>
@@ -5645,7 +5648,7 @@
       </c>
       <c r="G8" s="97"/>
     </row>
-    <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="103">
         <v>5</v>
       </c>
@@ -5658,14 +5661,14 @@
       <c r="D9" s="103">
         <v>3</v>
       </c>
-      <c r="E9" s="103">
-        <v>1</v>
+      <c r="E9" s="120">
+        <v>44198</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="103">
         <v>6</v>
       </c>
@@ -5688,7 +5691,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="103">
         <v>7</v>
       </c>
@@ -5696,7 +5699,7 @@
         <v>105</v>
       </c>
       <c r="C11" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D11" s="103">
         <v>8</v>
@@ -5708,7 +5711,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="89.25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="98" x14ac:dyDescent="0.15">
       <c r="A12" s="103">
         <v>8</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>106</v>
       </c>
       <c r="C12" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D12" s="103">
         <v>13</v>
@@ -5731,7 +5734,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A13" s="103">
         <v>9</v>
       </c>
@@ -5739,7 +5742,7 @@
         <v>107</v>
       </c>
       <c r="C13" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D13" s="103">
         <v>21</v>
@@ -5751,7 +5754,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="98">
         <v>10</v>
       </c>
@@ -5759,7 +5762,7 @@
         <v>108</v>
       </c>
       <c r="C14" s="98" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="98">
         <v>8</v>
@@ -5772,7 +5775,7 @@
       </c>
       <c r="G14" s="100"/>
     </row>
-    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="56" x14ac:dyDescent="0.15">
       <c r="A15" s="103">
         <v>11</v>
       </c>
@@ -5792,7 +5795,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="103">
         <v>12</v>
       </c>
@@ -5800,7 +5803,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="103">
         <v>13</v>
@@ -5812,7 +5815,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="42" x14ac:dyDescent="0.15">
       <c r="A17" s="103">
         <v>13</v>
       </c>
@@ -5832,7 +5835,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="98" x14ac:dyDescent="0.15">
       <c r="A18" s="103">
         <v>14</v>
       </c>
@@ -5840,7 +5843,7 @@
         <v>115</v>
       </c>
       <c r="C18" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="103">
         <v>1</v>
@@ -5855,7 +5858,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A19" s="103">
         <v>15</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>116</v>
       </c>
       <c r="C19" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D19" s="103">
         <v>12</v>
@@ -5878,7 +5881,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="56" x14ac:dyDescent="0.15">
       <c r="A20" s="103">
         <v>16</v>
       </c>
@@ -5886,7 +5889,7 @@
         <v>117</v>
       </c>
       <c r="C20" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D20" s="103">
         <v>1</v>
@@ -5898,7 +5901,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.15">
       <c r="A21" s="103">
         <v>17</v>
       </c>
@@ -5906,7 +5909,7 @@
         <v>118</v>
       </c>
       <c r="C21" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D21" s="103">
         <v>12</v>
@@ -5918,7 +5921,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="100" customFormat="1" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="100" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="103">
         <v>18</v>
       </c>
@@ -5932,14 +5935,14 @@
         <v>15</v>
       </c>
       <c r="E22" s="103">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="113" t="s">
         <v>119</v>
       </c>
       <c r="G22" s="31"/>
     </row>
-    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="42" x14ac:dyDescent="0.15">
       <c r="A23" s="103">
         <v>19</v>
       </c>
@@ -5947,7 +5950,7 @@
         <v>126</v>
       </c>
       <c r="C23" s="103" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D23" s="103">
         <v>21</v>
@@ -5959,7 +5962,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="103">
         <v>20</v>
       </c>
@@ -5967,7 +5970,7 @@
         <v>127</v>
       </c>
       <c r="C24" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" s="103">
         <v>12</v>
@@ -5979,13 +5982,13 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.15">
       <c r="J37" s="73"/>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.15">
       <c r="G42" s="73"/>
     </row>
-    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 A54:G163 B47:F52 B33:F44 G33:G41 A33:A52 A4:G24">
@@ -6054,13 +6057,13 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>101600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>1057275</xdr:colOff>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>333375</xdr:rowOff>
+                    <xdr:rowOff>330200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6078,32 +6081,32 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="251" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.73046875" customWidth="1"/>
-    <col min="2" max="3" width="8.73046875" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" customWidth="1"/>
-    <col min="5" max="5" width="14.3984375" customWidth="1"/>
-    <col min="6" max="6" width="15.73046875" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="5.3984375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.265625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="4.265625" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="6.73046875" hidden="1" customWidth="1"/>
-    <col min="14" max="16" width="9.1328125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="10.3984375" hidden="1" customWidth="1"/>
-    <col min="18" max="256" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="5.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="18" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6118,7 +6121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -6136,7 +6139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="F5" t="s">
         <v>42</v>
       </c>
@@ -6148,7 +6151,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6174,7 +6177,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="117">
         <f>D$4</f>
         <v>3</v>
@@ -6182,19 +6185,19 @@
       <c r="B8" s="117"/>
       <c r="D8" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Z8" s="36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,1,0,SprintCount,1)))</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -6207,43 +6210,43 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="55">
         <f ca="1">IF(D28="","",AVERAGE(LastEight))</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Z10" s="36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="55">
         <f ca="1">IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(LastEight,1),SMALL(LastEight,2),SMALL(LastEight,3))))</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Z11" s="36" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="55">
         <f ca="1">IF(M29="","",M28-M29)</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Z12" s="36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="F13" s="53" t="s">
         <v>52</v>
       </c>
@@ -6251,12 +6254,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -6265,7 +6268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -6274,7 +6277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -6290,7 +6293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18" s="117">
         <f>D$4</f>
         <v>3</v>
@@ -6298,32 +6301,32 @@
       <c r="B18" s="117"/>
       <c r="D18" s="56">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/D9+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D9,0)+SprintCount))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
         <v>63</v>
       </c>
       <c r="G19">
         <f ca="1">LastPlanned</f>
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="D20" s="56">
         <f ca="1">IF(D10="","",IF(LastRealized="",ROUNDUP(LastPlanned/D10+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D10,0)+SprintCount))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -6333,16 +6336,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="56">
         <f ca="1">IF(D11="","",IF(LastRealized="",ROUNDUP(LastPlanned/D11+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D11,0)+SprintCount))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -6351,25 +6354,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9+G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9+G17)+SprintCount,0)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9-G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9-G17)+SprintCount,0)))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="119" t="s">
         <v>24</v>
       </c>
@@ -6387,7 +6390,7 @@
       <c r="P26" s="119"/>
       <c r="Q26" s="119"/>
     </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" ht="26.65" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:17" s="3" customFormat="1" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="57" t="s">
         <v>13</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28" s="54">
         <v>1</v>
       </c>
@@ -6448,7 +6451,7 @@
         <v>92</v>
       </c>
       <c r="D28" s="2">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="E28" s="54">
         <f>B28</f>
@@ -6487,24 +6490,24 @@
       </c>
       <c r="O28" s="63">
         <f t="shared" ref="O28:O51" ca="1" si="5">D$9</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P28" s="63">
         <f t="shared" ref="P28:P51" ca="1" si="6">D$10</f>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q28" s="63">
         <f t="shared" ref="Q28:Q51" ca="1" si="7">D$11</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" s="54">
         <v>2</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" ref="B29:B51" si="8">IF(OR(B28="",C28=""),"",IF(D28="",IF(B28-C28&lt;=0,"",B28-C28),IF(B28-D28&lt;=0,"",B28-D28)))</f>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="C29" s="2">
         <v>102</v>
@@ -6516,11 +6519,11 @@
       </c>
       <c r="F29" s="52">
         <f t="shared" ref="F29:F34" si="9">IF(B29="",IF(B28="","",IF(D28="","",I28)),IF(AND(D28="",C28=""),"",IF(AND(D28="",C28&lt;&gt;""),IF(I28&gt;F28,F28,I28),F28-D28)))</f>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="G29" s="52">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="H29" s="52">
         <f t="shared" si="1"/>
@@ -6532,15 +6535,15 @@
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="L29" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="M29" s="52">
         <f ca="1">IF(L29=L28,"",L29)</f>
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="N29" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6548,24 +6551,24 @@
       </c>
       <c r="O29" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P29" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q29" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30" s="54">
         <v>3</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="8"/>
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2">
         <v>114</v>
@@ -6585,23 +6588,23 @@
       </c>
       <c r="H30" s="52">
         <f t="shared" si="1"/>
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="I30" s="52">
         <f>IF(B30="",IF(B29="","",IF(D29="","",F29-D29)),IF(AND(C29="",D29=""),"",IF(AND(D29="",C29&lt;&gt;""),IF(I29&gt;F29,I29-C29,F29-C29),B$28-B30-SUM(D$28:D29))))</f>
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="L30" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>213.99999999999997</v>
+        <v>128</v>
       </c>
       <c r="M30" s="52">
         <f t="shared" ref="M30:M51" ca="1" si="10">IF(L30=L29,"",L30)</f>
-        <v>213.99999999999997</v>
+        <v>128</v>
       </c>
       <c r="N30" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6609,18 +6612,18 @@
       </c>
       <c r="O30" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P30" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q30" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31" s="54">
         <v>4</v>
       </c>
@@ -6653,11 +6656,11 @@
       </c>
       <c r="L31" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>167.99999999999997</v>
+        <v>39</v>
       </c>
       <c r="M31" s="52">
         <f t="shared" ca="1" si="10"/>
-        <v>167.99999999999997</v>
+        <v>39</v>
       </c>
       <c r="N31" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6665,18 +6668,18 @@
       </c>
       <c r="O31" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P31" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q31" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32" s="54"/>
       <c r="B32" s="2" t="str">
         <f>IF(OR(B31="",C31=""),"",IF(D31="",IF(B31-C31&lt;=0,"",B31-C31),IF(B31-D31&lt;=0,"",B31-D31)))</f>
@@ -6722,18 +6725,18 @@
       </c>
       <c r="O32" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P32" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q32" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33" s="54"/>
       <c r="B33" s="2" t="str">
         <f>IF(OR(B32="",C32=""),"",IF(D32="",IF(B32-C32&lt;=0,"",B32-C32),IF(B32-D32&lt;=0,"",B32-D32)))</f>
@@ -6779,18 +6782,18 @@
       </c>
       <c r="O33" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P33" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q33" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34" s="54"/>
       <c r="B34" s="2" t="str">
         <f>IF(OR(B33="",C33=""),"",IF(D33="",IF(B33-C33&lt;=0,"",B33-C33),IF(B33-D33&lt;=0,"",B33-D33)))</f>
@@ -6836,18 +6839,18 @@
       </c>
       <c r="O34" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P34" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q34" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35" s="54"/>
       <c r="B35" s="2" t="str">
         <f t="shared" si="8"/>
@@ -6893,18 +6896,18 @@
       </c>
       <c r="O35" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P35" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q35" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36" s="54"/>
       <c r="B36" s="2" t="str">
         <f t="shared" si="8"/>
@@ -6950,18 +6953,18 @@
       </c>
       <c r="O36" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P36" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q36" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" s="54"/>
       <c r="B37" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7007,18 +7010,18 @@
       </c>
       <c r="O37" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P37" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q37" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A38" s="54"/>
       <c r="B38" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7064,18 +7067,18 @@
       </c>
       <c r="O38" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P38" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q38" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39" s="54"/>
       <c r="B39" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7121,18 +7124,18 @@
       </c>
       <c r="O39" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P39" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q39" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40" s="54"/>
       <c r="B40" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7177,18 +7180,18 @@
       </c>
       <c r="O40" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P40" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q40" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A41" s="54"/>
       <c r="B41" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7233,18 +7236,18 @@
       </c>
       <c r="O41" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P41" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q41" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A42" s="54"/>
       <c r="B42" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7289,18 +7292,18 @@
       </c>
       <c r="O42" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P42" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q42" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A43" s="54"/>
       <c r="B43" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7345,18 +7348,18 @@
       </c>
       <c r="O43" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P43" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q43" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A44" s="54"/>
       <c r="B44" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7401,18 +7404,18 @@
       </c>
       <c r="O44" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P44" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q44" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A45" s="54"/>
       <c r="B45" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7457,18 +7460,18 @@
       </c>
       <c r="O45" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P45" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q45" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A46" s="54"/>
       <c r="B46" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7513,18 +7516,18 @@
       </c>
       <c r="O46" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P46" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q46" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A47" s="54"/>
       <c r="B47" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7569,18 +7572,18 @@
       </c>
       <c r="O47" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P47" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q47" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A48" s="54"/>
       <c r="B48" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7625,18 +7628,18 @@
       </c>
       <c r="O48" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P48" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q48" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A49" s="54"/>
       <c r="B49" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7681,18 +7684,18 @@
       </c>
       <c r="O49" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P49" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q49" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A50" s="54"/>
       <c r="B50" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7737,18 +7740,18 @@
       </c>
       <c r="O50" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P50" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q50" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A51" s="54"/>
       <c r="B51" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7793,15 +7796,15 @@
       </c>
       <c r="O51" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P51" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="Q51" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -7842,20 +7845,20 @@
       <selection pane="bottomLeft" activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="43.3984375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="13.73046875" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.73046875" style="33" customWidth="1"/>
-    <col min="5" max="5" width="6.3984375" style="32" customWidth="1"/>
-    <col min="6" max="30" width="4.3984375" style="32" customWidth="1"/>
-    <col min="31" max="31" width="9.1328125" style="33"/>
-    <col min="32" max="32" width="41.1328125" style="33" customWidth="1"/>
-    <col min="33" max="16384" width="9.1328125" style="33"/>
+    <col min="1" max="1" width="43.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="32" customWidth="1"/>
+    <col min="6" max="30" width="4.33203125" style="32" customWidth="1"/>
+    <col min="31" max="31" width="9.1640625" style="33"/>
+    <col min="32" max="32" width="41.1640625" style="33" customWidth="1"/>
+    <col min="33" max="16384" width="9.1640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="64">
         <v>1</v>
       </c>
@@ -7887,7 +7890,7 @@
       <c r="AC1" s="33"/>
       <c r="AD1" s="33"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
@@ -7915,7 +7918,7 @@
       <c r="AC2" s="33"/>
       <c r="AD2" s="33"/>
     </row>
-    <row r="9" spans="1:32" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -7955,7 +7958,7 @@
       <c r="AC9" s="68"/>
       <c r="AD9" s="68"/>
     </row>
-    <row r="10" spans="1:32" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A10" s="66" t="s">
         <v>29</v>
       </c>
@@ -8073,7 +8076,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -8190,7 +8193,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:32" customFormat="1" ht="13.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
         <v>26</v>
       </c>
@@ -8300,7 +8303,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:32" customFormat="1" ht="13.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13" s="53" t="s">
         <v>27</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A14" s="66" t="s">
         <v>7</v>
       </c>
@@ -8505,7 +8508,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -8536,7 +8539,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -8566,7 +8569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -8604,7 +8607,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A19" s="31"/>
       <c r="C19"/>
       <c r="AC19" s="32" t="str">
@@ -8645,7 +8648,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
       <c r="B20"/>
       <c r="C20"/>
       <c r="AC20" s="32" t="str">
@@ -8657,7 +8660,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="31"/>
       <c r="C21"/>
       <c r="AC21" s="32" t="str">
@@ -8669,7 +8672,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A22" s="31"/>
       <c r="C22"/>
       <c r="AC22" s="32" t="str">
@@ -8681,7 +8684,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="31"/>
       <c r="C23"/>
       <c r="AC23" s="32" t="str">
@@ -8693,7 +8696,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A24" s="31"/>
       <c r="C24"/>
       <c r="AC24" s="32" t="str">
@@ -8705,11 +8708,11 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A25" s="31"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A26" s="31"/>
       <c r="C26"/>
       <c r="AC26" s="32" t="str">
@@ -8721,7 +8724,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A27" s="31"/>
       <c r="C27"/>
       <c r="AC27" s="32" t="str">
@@ -8733,7 +8736,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A28" s="31"/>
       <c r="C28"/>
       <c r="AC28" s="32" t="str">
@@ -8745,7 +8748,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A29" s="31"/>
       <c r="C29"/>
       <c r="AC29" s="32" t="str">
@@ -8757,7 +8760,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A30" s="31"/>
       <c r="C30"/>
       <c r="AC30" s="32" t="str">
@@ -8769,7 +8772,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A31" s="31"/>
       <c r="C31"/>
       <c r="AC31" s="32" t="str">
@@ -8781,7 +8784,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A32" s="31"/>
       <c r="C32"/>
       <c r="AC32" s="32" t="str">
@@ -8793,7 +8796,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A33" s="31"/>
       <c r="C33"/>
       <c r="AC33" s="32" t="str">
@@ -8805,7 +8808,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A34" s="31"/>
       <c r="C34"/>
       <c r="AC34" s="32" t="str">
@@ -8817,11 +8820,11 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A35" s="31"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A36" s="31"/>
       <c r="C36"/>
       <c r="AC36" s="32" t="str">
@@ -8833,7 +8836,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A37" s="31"/>
       <c r="C37"/>
       <c r="AC37" s="32" t="str">
@@ -8845,7 +8848,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A38" s="31"/>
       <c r="C38"/>
       <c r="AC38" s="32" t="str">
@@ -8857,7 +8860,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A39" s="31"/>
       <c r="C39"/>
       <c r="AC39" s="32" t="str">
@@ -8869,7 +8872,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A40" s="31"/>
       <c r="C40"/>
       <c r="AC40" s="32" t="str">
@@ -8881,7 +8884,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A41" s="31"/>
       <c r="C41"/>
       <c r="D41" s="33" t="str">
@@ -8901,7 +8904,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C42"/>
       <c r="D42" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8920,7 +8923,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C43"/>
       <c r="D43" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8939,7 +8942,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C44"/>
       <c r="D44" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8958,7 +8961,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C45"/>
       <c r="D45" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8977,7 +8980,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C46"/>
       <c r="D46" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8996,7 +8999,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C47"/>
       <c r="D47" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9015,7 +9018,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
       <c r="C48"/>
       <c r="D48" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9034,7 +9037,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C49"/>
       <c r="D49" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9053,7 +9056,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C50"/>
       <c r="D50" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9072,7 +9075,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C51"/>
       <c r="D51" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9091,7 +9094,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C52"/>
       <c r="D52" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9110,7 +9113,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C53"/>
       <c r="D53" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9129,7 +9132,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C54"/>
       <c r="D54" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9148,7 +9151,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C55"/>
       <c r="D55" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9167,7 +9170,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C56"/>
       <c r="D56" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9186,7 +9189,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C57"/>
       <c r="D57" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9205,7 +9208,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C58"/>
       <c r="D58" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9224,7 +9227,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C59"/>
       <c r="D59" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9243,7 +9246,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C60"/>
       <c r="D60" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9262,7 +9265,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C61"/>
       <c r="D61" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9281,7 +9284,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C62"/>
       <c r="D62" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9388,7 +9391,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C63"/>
       <c r="D63" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9495,80 +9498,80 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:30" x14ac:dyDescent="0.15">
       <c r="C64"/>
       <c r="D64" s="33" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C65"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C66"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C67"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C68"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C69"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C70"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C71"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C72"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C73"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C74"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C75"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C76"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C77"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C78"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C79"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C80"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C81"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C82"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C83"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C84"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C85"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C86"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C87"/>
     </row>
   </sheetData>
@@ -9611,13 +9614,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>101600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>2314575</xdr:colOff>
+                    <xdr:colOff>2311400</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9633,13 +9636,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2590800</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>101600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9662,20 +9665,20 @@
       <selection pane="bottomLeft" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="38.3984375" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.73046875" customWidth="1"/>
-    <col min="4" max="4" width="10.73046875" customWidth="1"/>
-    <col min="5" max="5" width="6.3984375" style="2" customWidth="1"/>
-    <col min="6" max="30" width="4.3984375" style="2" customWidth="1"/>
-    <col min="31" max="31" width="8.73046875" customWidth="1"/>
-    <col min="32" max="32" width="45.1328125" customWidth="1"/>
-    <col min="33" max="256" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="2" customWidth="1"/>
+    <col min="6" max="30" width="4.33203125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="8.6640625" customWidth="1"/>
+    <col min="32" max="32" width="45.1640625" customWidth="1"/>
+    <col min="33" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="30">
         <v>1</v>
       </c>
@@ -9707,7 +9710,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -9735,7 +9738,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="9" spans="1:32" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>12</v>
       </c>
@@ -9775,7 +9778,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="21"/>
     </row>
-    <row r="10" spans="1:32" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -10009,7 +10012,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="13.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="53" t="s">
         <v>26</v>
       </c>
@@ -10119,7 +10122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="13.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13" s="53" t="s">
         <v>27</v>
       </c>
@@ -10208,7 +10211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>7</v>
       </c>
@@ -10324,7 +10327,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" ht="42" x14ac:dyDescent="0.15">
       <c r="D15" t="str">
         <f t="shared" ref="D15:D59" si="4">IF(A15&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10337,7 +10340,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
       <c r="D16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10355,7 +10358,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D17" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10373,7 +10376,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D18" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10391,7 +10394,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D19" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10409,7 +10412,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D20" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10427,7 +10430,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D21" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10445,7 +10448,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D22" t="str">
         <f>IF(A22&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10463,7 +10466,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D23" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10481,7 +10484,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D24" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10499,7 +10502,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D25" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10517,7 +10520,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D26" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10535,7 +10538,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D27" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10553,7 +10556,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D28" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10571,7 +10574,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D29" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10589,7 +10592,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D30" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10607,7 +10610,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D31" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10625,7 +10628,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D32" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10643,7 +10646,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D33" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10661,7 +10664,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D34" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10679,7 +10682,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D35" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10697,7 +10700,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D36" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10715,7 +10718,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D37" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10733,7 +10736,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D38" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10751,7 +10754,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D39" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10769,7 +10772,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D40" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10787,7 +10790,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D41" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10805,7 +10808,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D42" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10823,7 +10826,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D43" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10841,7 +10844,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10859,7 +10862,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D45" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10877,7 +10880,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D46" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10895,7 +10898,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D47" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10913,7 +10916,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D48" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10931,7 +10934,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D49" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10949,7 +10952,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D50" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10967,7 +10970,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D51" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10985,7 +10988,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D52" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11003,7 +11006,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D53" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11021,7 +11024,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D54" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11039,7 +11042,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D55" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11057,7 +11060,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D56" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11075,7 +11078,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D57" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11093,7 +11096,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D58" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11199,7 +11202,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D59" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11305,7 +11308,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="4:30" x14ac:dyDescent="0.15">
       <c r="D64" t="str">
         <f>IF(A64&lt;&gt;"","Planned","")</f>
         <v/>
@@ -11359,13 +11362,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>101600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>1981200</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11381,13 +11384,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2286000</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>104775</xdr:rowOff>
+                    <xdr:rowOff>101600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:colOff>254000</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11411,18 +11414,18 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="9.1328125" style="33"/>
-    <col min="4" max="4" width="32.73046875" style="33" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" style="33"/>
-    <col min="6" max="6" width="32.73046875" style="33" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" style="33"/>
-    <col min="8" max="8" width="41.73046875" style="33" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="33"/>
+    <col min="1" max="3" width="9.1640625" style="33"/>
+    <col min="4" max="4" width="32.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="33"/>
+    <col min="6" max="6" width="32.6640625" style="33" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="33"/>
+    <col min="8" max="8" width="41.6640625" style="33" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="79" t="s">
         <v>95</v>
       </c>
@@ -11438,7 +11441,7 @@
       <c r="E1" s="81"/>
       <c r="F1" s="82"/>
     </row>
-    <row r="2" spans="1:8" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A2" s="83" t="s">
         <v>97</v>
       </c>
@@ -11453,7 +11456,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="85"/>
       <c r="B3" s="77"/>
       <c r="C3" s="77"/>
@@ -11461,7 +11464,7 @@
       <c r="E3" s="77"/>
       <c r="F3" s="86"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="87"/>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
@@ -11469,7 +11472,7 @@
       <c r="E4" s="78"/>
       <c r="F4" s="88"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C15)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11480,7 +11483,7 @@
       <c r="E5" s="75"/>
       <c r="F5" s="94"/>
     </row>
-    <row r="6" spans="1:8" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="89" t="s">
         <v>94</v>
       </c>
@@ -11496,8 +11499,8 @@
       </c>
       <c r="F6" s="92"/>
     </row>
-    <row r="8" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="1:8" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="79" t="s">
         <v>95</v>
       </c>
@@ -11513,7 +11516,7 @@
       <c r="E9" s="81"/>
       <c r="F9" s="82"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="83" t="s">
         <v>97</v>
       </c>
@@ -11525,7 +11528,7 @@
       <c r="E10" s="76"/>
       <c r="F10" s="84"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="85"/>
       <c r="B11" s="77"/>
       <c r="C11" s="77"/>
@@ -11533,7 +11536,7 @@
       <c r="E11" s="77"/>
       <c r="F11" s="86"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="87"/>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
@@ -11541,7 +11544,7 @@
       <c r="E12" s="78"/>
       <c r="F12" s="88"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C16)</f>
         <v>Responsible Person: Tina Tester</v>
@@ -11552,7 +11555,7 @@
       <c r="E13" s="75"/>
       <c r="F13" s="94"/>
     </row>
-    <row r="14" spans="1:8" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="89" t="s">
         <v>94</v>
       </c>
@@ -11568,8 +11571,8 @@
       </c>
       <c r="F14" s="92"/>
     </row>
-    <row r="16" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="79" t="s">
         <v>95</v>
       </c>
@@ -11585,7 +11588,7 @@
       <c r="E17" s="81"/>
       <c r="F17" s="82"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="83" t="s">
         <v>97</v>
       </c>
@@ -11597,7 +11600,7 @@
       <c r="E18" s="76"/>
       <c r="F18" s="84"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="85"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77"/>
@@ -11605,7 +11608,7 @@
       <c r="E19" s="77"/>
       <c r="F19" s="86"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="87"/>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
@@ -11613,7 +11616,7 @@
       <c r="E20" s="78"/>
       <c r="F20" s="88"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C17)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11624,7 +11627,7 @@
       <c r="E21" s="75"/>
       <c r="F21" s="94"/>
     </row>
-    <row r="22" spans="1:6" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="89" t="s">
         <v>94</v>
       </c>
@@ -11640,8 +11643,8 @@
       </c>
       <c r="F22" s="92"/>
     </row>
-    <row r="24" spans="1:6" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:6" ht="13.15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="79" t="s">
         <v>95</v>
       </c>
@@ -11657,7 +11660,7 @@
       <c r="E25" s="81"/>
       <c r="F25" s="82"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="83" t="s">
         <v>97</v>
       </c>
@@ -11669,7 +11672,7 @@
       <c r="E26" s="76"/>
       <c r="F26" s="84"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="85"/>
       <c r="B27" s="77"/>
       <c r="C27" s="77"/>
@@ -11677,7 +11680,7 @@
       <c r="E27" s="77"/>
       <c r="F27" s="86"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="87"/>
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
@@ -11685,7 +11688,7 @@
       <c r="E28" s="78"/>
       <c r="F28" s="88"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C18)</f>
         <v xml:space="preserve">Responsible Person: </v>
@@ -11696,7 +11699,7 @@
       <c r="E29" s="75"/>
       <c r="F29" s="94"/>
     </row>
-    <row r="30" spans="1:6" ht="25.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="89" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Updated burndown chart to show sprint 2 progress.
May need to update sprint 3's planned work as well.
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmabrothers/Documents/SubscriptionTracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AD9F59-0E2E-4746-BDC1-D580375D2052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CACCB58-AC24-488E-A986-D23D58E2DCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="32580" windowHeight="20200" tabRatio="522" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="7" r:id="rId1"/>
@@ -1546,6 +1546,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1554,9 +1557,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1840,7 +1840,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1933,7 +1933,7 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1969,7 +1969,7 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,7 +2050,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2098,16 +2098,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>306</c:v>
+                  <c:v>294.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217</c:v>
+                  <c:v>239.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128</c:v>
+                  <c:v>184.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>129.66666666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2146,7 +2146,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2349,7 +2349,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2485,6 +2485,9 @@
                 <c:pt idx="0">
                   <c:v>89</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2533,13 +2536,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2575,13 +2578,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2617,13 +2620,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2840,7 +2843,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3414,7 +3417,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4014,13 +4017,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>1054100</xdr:colOff>
+          <xdr:colOff>1051560</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>330200</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4052,19 +4055,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Sort Product Backlog</a:t>
               </a:r>
@@ -4207,13 +4210,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>2311400</xdr:colOff>
+          <xdr:colOff>2308860</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4245,19 +4248,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Sort Sprint Tasks</a:t>
               </a:r>
@@ -4276,13 +4279,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2590800</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4314,19 +4317,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Update Task Slips</a:t>
               </a:r>
@@ -4388,13 +4391,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>266700</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>1981200</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4426,19 +4429,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Sort Sprint Tasks</a:t>
               </a:r>
@@ -4457,13 +4460,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>2286000</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>254000</xdr:colOff>
+          <xdr:colOff>251460</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4495,19 +4498,19 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-NZ" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Arial" pitchFamily="2" charset="0"/>
-                  <a:cs typeface="Arial" pitchFamily="2" charset="0"/>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
                 </a:rPr>
                 <a:t>Update Task Slips</a:t>
               </a:r>
@@ -4877,7 +4880,7 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
@@ -4885,17 +4888,17 @@
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="59.1640625" customWidth="1"/>
+    <col min="8" max="8" width="59.109375" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
@@ -4923,7 +4926,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -4947,7 +4950,7 @@
       <c r="G4" s="46"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2</v>
       </c>
@@ -4971,7 +4974,7 @@
       <c r="G5" s="47"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="39"/>
       <c r="C6" s="22" t="str">
@@ -4990,7 +4993,7 @@
       <c r="G6" s="47"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="39"/>
       <c r="C7" s="22" t="str">
@@ -5009,7 +5012,7 @@
       <c r="G7" s="47"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="39"/>
       <c r="C8" s="22" t="str">
@@ -5028,7 +5031,7 @@
       <c r="G8" s="47"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="39"/>
       <c r="C9" s="22" t="str">
@@ -5047,7 +5050,7 @@
       <c r="G9" s="47"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="40"/>
       <c r="C10" s="41" t="str">
@@ -5066,17 +5069,17 @@
       <c r="G10" s="48"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
@@ -5106,7 +5109,7 @@
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>1</v>
       </c>
@@ -5134,7 +5137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>2</v>
       </c>
@@ -5163,7 +5166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>3</v>
       </c>
@@ -5193,7 +5196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
@@ -5204,7 +5207,7 @@
       <c r="H19" s="28"/>
       <c r="I19" s="37"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="26"/>
       <c r="C20" s="27"/>
@@ -5215,7 +5218,7 @@
       <c r="H20" s="28"/>
       <c r="I20" s="37"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
@@ -5226,7 +5229,7 @@
       <c r="H21" s="28"/>
       <c r="I21" s="37"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
@@ -5237,7 +5240,7 @@
       <c r="H22" s="28"/>
       <c r="I22" s="37"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="str">
         <f t="shared" ref="A23:A30" si="3">IF(AND(B23&lt;&gt;"",C23&lt;&gt;""),A22+1,"")</f>
         <v/>
@@ -5263,7 +5266,7 @@
       <c r="H23" s="28"/>
       <c r="I23" s="37"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5289,7 +5292,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="37"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5315,7 +5318,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="37"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5341,7 +5344,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="37"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5367,7 +5370,7 @@
       <c r="H27" s="28"/>
       <c r="I27" s="37"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5393,7 +5396,7 @@
       <c r="H28" s="28"/>
       <c r="I28" s="37"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5419,7 +5422,7 @@
       <c r="H29" s="28"/>
       <c r="I29" s="37"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5445,7 +5448,7 @@
       <c r="H30" s="29"/>
       <c r="I30" s="38"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -5508,21 +5511,21 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="103"/>
+    <col min="1" max="1" width="9.109375" style="103"/>
     <col min="2" max="2" width="39.33203125" style="31" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="103" customWidth="1"/>
-    <col min="4" max="6" width="9.1640625" style="103"/>
+    <col min="4" max="6" width="9.109375" style="103"/>
     <col min="7" max="7" width="39.33203125" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="31"/>
+    <col min="8" max="16384" width="9.109375" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="76" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>5</v>
       </c>
@@ -5530,10 +5533,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" s="104"/>
     </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105" t="s">
         <v>21</v>
       </c>
@@ -5556,7 +5559,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="113" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="106.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="106">
         <v>1</v>
       </c>
@@ -5582,7 +5585,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="108">
         <v>2</v>
       </c>
@@ -5607,7 +5610,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="103">
         <v>3</v>
       </c>
@@ -5627,7 +5630,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" s="103">
         <v>4</v>
       </c>
@@ -5648,7 +5651,7 @@
       </c>
       <c r="G8" s="97"/>
     </row>
-    <row r="9" spans="1:9" ht="42" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A9" s="103">
         <v>5</v>
       </c>
@@ -5661,14 +5664,14 @@
       <c r="D9" s="103">
         <v>3</v>
       </c>
-      <c r="E9" s="120">
+      <c r="E9" s="117">
         <v>44198</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="103">
         <v>6</v>
       </c>
@@ -5691,7 +5694,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="103">
         <v>7</v>
       </c>
@@ -5711,7 +5714,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="98" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A12" s="103">
         <v>8</v>
       </c>
@@ -5734,7 +5737,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A13" s="103">
         <v>9</v>
       </c>
@@ -5754,7 +5757,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="98">
         <v>10</v>
       </c>
@@ -5775,7 +5778,7 @@
       </c>
       <c r="G14" s="100"/>
     </row>
-    <row r="15" spans="1:9" ht="56" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="103">
         <v>11</v>
       </c>
@@ -5795,7 +5798,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="103">
         <v>12</v>
       </c>
@@ -5815,7 +5818,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="103">
         <v>13</v>
       </c>
@@ -5835,7 +5838,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="98" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A18" s="103">
         <v>14</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A19" s="103">
         <v>15</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A20" s="103">
         <v>16</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21" s="103">
         <v>17</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="100" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" s="100" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="103">
         <v>18</v>
       </c>
@@ -5942,7 +5945,7 @@
       </c>
       <c r="G22" s="31"/>
     </row>
-    <row r="23" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A23" s="103">
         <v>19</v>
       </c>
@@ -5950,7 +5953,7 @@
         <v>126</v>
       </c>
       <c r="C23" s="103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="103">
         <v>21</v>
@@ -5962,7 +5965,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A24" s="103">
         <v>20</v>
       </c>
@@ -5982,13 +5985,13 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.15">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="J37" s="73"/>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.15">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" s="73"/>
     </row>
-    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="53" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G44:G52 C45:C46 A54:G163 B47:F52 B33:F44 G33:G41 A33:A52 A4:G24">
@@ -6057,13 +6060,13 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>1054100</xdr:colOff>
+                    <xdr:colOff>1051560</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>330200</xdr:rowOff>
+                    <xdr:rowOff>327660</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6081,32 +6084,32 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="251" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="96" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
     <col min="2" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="5.33203125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="4.33203125" hidden="1" customWidth="1"/>
     <col min="11" max="13" width="6.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="16" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="9.109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
     <col min="18" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6121,7 +6124,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -6136,10 +6139,10 @@
       </c>
       <c r="G4" s="52">
         <f>IF(COUNT(D28:D51)=0,1,COUNT(D28:D51)+1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>42</v>
       </c>
@@ -6151,7 +6154,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6160,13 +6163,13 @@
       </c>
       <c r="G6" s="52">
         <f>TrendSprintCount-TrendOffset</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z6" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6177,27 +6180,27 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A8" s="117">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="118">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B8" s="117"/>
+      <c r="B8" s="118"/>
       <c r="D8" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Z8" s="36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,1,0,SprintCount,1)))</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
@@ -6210,43 +6213,43 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="55">
         <f ca="1">IF(D28="","",AVERAGE(LastEight))</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Z10" s="36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="55">
         <f ca="1">IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(LastEight,1),SMALL(LastEight,2),SMALL(LastEight,3))))</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Z11" s="36" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="55">
         <f ca="1">IF(M29="","",M28-M29)</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Z12" s="36" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F13" s="53" t="s">
         <v>52</v>
       </c>
@@ -6254,12 +6257,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -6277,7 +6280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -6290,43 +6293,43 @@
       </c>
       <c r="G17">
         <f>IF(OR(D28="",D29=""),1,STDEV(D28:D51))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A18" s="117">
+        <v>48.083261120685229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="118">
         <f>D$4</f>
         <v>3</v>
       </c>
-      <c r="B18" s="117"/>
+      <c r="B18" s="118"/>
       <c r="D18" s="56">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/D9+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D9,0)+SprintCount))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
         <v>63</v>
       </c>
       <c r="G19">
         <f ca="1">LastPlanned</f>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="D20" s="56">
         <f ca="1">IF(D10="","",IF(LastRealized="",ROUNDUP(LastPlanned/D10+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D10,0)+SprintCount))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
         <v>64</v>
@@ -6336,16 +6339,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="56">
         <f ca="1">IF(D11="","",IF(LastRealized="",ROUNDUP(LastPlanned/D11+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D11,0)+SprintCount))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -6354,7 +6357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -6363,34 +6366,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9-G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9-G17)+SprintCount,0)))</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F26" s="119" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="119"/>
-      <c r="H26" s="119"/>
-      <c r="I26" s="119"/>
-      <c r="J26" s="119"/>
-      <c r="K26" s="119"/>
-      <c r="L26" s="119"/>
-      <c r="M26" s="119"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="119" t="s">
+      <c r="G26" s="120"/>
+      <c r="H26" s="120"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="120"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="120"/>
+      <c r="M26" s="120"/>
+      <c r="N26" s="120"/>
+      <c r="O26" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="P26" s="119"/>
-      <c r="Q26" s="119"/>
-    </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="P26" s="120"/>
+      <c r="Q26" s="120"/>
+    </row>
+    <row r="27" spans="1:17" s="3" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="57" t="s">
         <v>13</v>
       </c>
@@ -6409,10 +6412,10 @@
       <c r="F27" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="118" t="s">
+      <c r="G27" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="118"/>
+      <c r="H27" s="119"/>
       <c r="I27" s="60" t="s">
         <v>36</v>
       </c>
@@ -6439,7 +6442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="54">
         <v>1</v>
       </c>
@@ -6478,11 +6481,11 @@
       </c>
       <c r="L28" s="52">
         <f t="shared" ref="L28:L51" ca="1" si="3">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28)&lt;N28,N28,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28))</f>
-        <v>306</v>
+        <v>294.66666666666663</v>
       </c>
       <c r="M28" s="52">
         <f ca="1">L28</f>
-        <v>306</v>
+        <v>294.66666666666663</v>
       </c>
       <c r="N28" s="52">
         <f t="shared" ref="N28:N51" ca="1" si="4">OFFSET($I$27,TrendSprintCount,0,1,1)</f>
@@ -6490,18 +6493,18 @@
       </c>
       <c r="O28" s="63">
         <f t="shared" ref="O28:O51" ca="1" si="5">D$9</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P28" s="63">
         <f t="shared" ref="P28:P51" ca="1" si="6">D$10</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q28" s="63">
         <f t="shared" ref="Q28:Q51" ca="1" si="7">D$11</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="54">
         <v>2</v>
       </c>
@@ -6512,7 +6515,9 @@
       <c r="C29" s="2">
         <v>102</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>21</v>
+      </c>
       <c r="E29" s="54">
         <f>IF(B29="","",IF(D28="",E28,B29+SUM(D$28:D28)))</f>
         <v>306</v>
@@ -6539,11 +6544,11 @@
       </c>
       <c r="L29" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>217</v>
+        <v>239.66666666666663</v>
       </c>
       <c r="M29" s="52">
         <f ca="1">IF(L29=L28,"",L29)</f>
-        <v>217</v>
+        <v>239.66666666666663</v>
       </c>
       <c r="N29" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6551,24 +6556,24 @@
       </c>
       <c r="O29" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P29" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q29" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="54">
         <v>3</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="8"/>
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="C30" s="2">
         <v>114</v>
@@ -6580,31 +6585,31 @@
       </c>
       <c r="F30" s="52">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="G30" s="52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="H30" s="52">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="I30" s="52">
         <f>IF(B30="",IF(B29="","",IF(D29="","",F29-D29)),IF(AND(C29="",D29=""),"",IF(AND(D29="",C29&lt;&gt;""),IF(I29&gt;F29,I29-C29,F29-C29),B$28-B30-SUM(D$28:D29))))</f>
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="L30" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>128</v>
+        <v>184.66666666666663</v>
       </c>
       <c r="M30" s="52">
         <f t="shared" ref="M30:M51" ca="1" si="10">IF(L30=L29,"",L30)</f>
-        <v>128</v>
+        <v>184.66666666666663</v>
       </c>
       <c r="N30" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6612,18 +6617,18 @@
       </c>
       <c r="O30" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P30" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q30" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="54">
         <v>4</v>
       </c>
@@ -6656,11 +6661,11 @@
       </c>
       <c r="L31" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>129.66666666666663</v>
       </c>
       <c r="M31" s="52">
         <f t="shared" ca="1" si="10"/>
-        <v>39</v>
+        <v>129.66666666666663</v>
       </c>
       <c r="N31" s="52">
         <f t="shared" ca="1" si="4"/>
@@ -6668,18 +6673,18 @@
       </c>
       <c r="O31" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P31" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q31" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="2" t="str">
         <f>IF(OR(B31="",C31=""),"",IF(D31="",IF(B31-C31&lt;=0,"",B31-C31),IF(B31-D31&lt;=0,"",B31-D31)))</f>
@@ -6725,18 +6730,18 @@
       </c>
       <c r="O32" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P32" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q32" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="54"/>
       <c r="B33" s="2" t="str">
         <f>IF(OR(B32="",C32=""),"",IF(D32="",IF(B32-C32&lt;=0,"",B32-C32),IF(B32-D32&lt;=0,"",B32-D32)))</f>
@@ -6782,18 +6787,18 @@
       </c>
       <c r="O33" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P33" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q33" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="54"/>
       <c r="B34" s="2" t="str">
         <f>IF(OR(B33="",C33=""),"",IF(D33="",IF(B33-C33&lt;=0,"",B33-C33),IF(B33-D33&lt;=0,"",B33-D33)))</f>
@@ -6839,18 +6844,18 @@
       </c>
       <c r="O34" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P34" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q34" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="54"/>
       <c r="B35" s="2" t="str">
         <f t="shared" si="8"/>
@@ -6896,18 +6901,18 @@
       </c>
       <c r="O35" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P35" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q35" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="54"/>
       <c r="B36" s="2" t="str">
         <f t="shared" si="8"/>
@@ -6953,18 +6958,18 @@
       </c>
       <c r="O36" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P36" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q36" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="54"/>
       <c r="B37" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7010,18 +7015,18 @@
       </c>
       <c r="O37" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P37" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q37" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="54"/>
       <c r="B38" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7067,18 +7072,18 @@
       </c>
       <c r="O38" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P38" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q38" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="54"/>
       <c r="B39" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7124,18 +7129,18 @@
       </c>
       <c r="O39" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P39" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q39" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="54"/>
       <c r="B40" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7180,18 +7185,18 @@
       </c>
       <c r="O40" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P40" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q40" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="54"/>
       <c r="B41" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7236,18 +7241,18 @@
       </c>
       <c r="O41" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P41" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q41" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="54"/>
       <c r="B42" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7292,18 +7297,18 @@
       </c>
       <c r="O42" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P42" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q42" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="54"/>
       <c r="B43" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7348,18 +7353,18 @@
       </c>
       <c r="O43" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P43" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q43" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="54"/>
       <c r="B44" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7404,18 +7409,18 @@
       </c>
       <c r="O44" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P44" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q44" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="54"/>
       <c r="B45" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7460,18 +7465,18 @@
       </c>
       <c r="O45" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P45" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q45" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="54"/>
       <c r="B46" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7516,18 +7521,18 @@
       </c>
       <c r="O46" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P46" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q46" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="54"/>
       <c r="B47" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7572,18 +7577,18 @@
       </c>
       <c r="O47" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P47" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q47" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="54"/>
       <c r="B48" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7628,18 +7633,18 @@
       </c>
       <c r="O48" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P48" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q48" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="54"/>
       <c r="B49" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7684,18 +7689,18 @@
       </c>
       <c r="O49" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P49" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q49" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="54"/>
       <c r="B50" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7740,18 +7745,18 @@
       </c>
       <c r="O50" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P50" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q50" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="54"/>
       <c r="B51" s="2" t="str">
         <f t="shared" si="8"/>
@@ -7796,15 +7801,15 @@
       </c>
       <c r="O51" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="P51" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="Q51" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -7845,7 +7850,7 @@
       <selection pane="bottomLeft" activeCell="AF17" sqref="AF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.33203125" style="33" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="32" customWidth="1"/>
@@ -7853,12 +7858,12 @@
     <col min="4" max="4" width="10.6640625" style="33" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="32" customWidth="1"/>
     <col min="6" max="30" width="4.33203125" style="32" customWidth="1"/>
-    <col min="31" max="31" width="9.1640625" style="33"/>
-    <col min="32" max="32" width="41.1640625" style="33" customWidth="1"/>
-    <col min="33" max="16384" width="9.1640625" style="33"/>
+    <col min="31" max="31" width="9.109375" style="33"/>
+    <col min="32" max="32" width="41.109375" style="33" customWidth="1"/>
+    <col min="33" max="16384" width="9.109375" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="64">
         <v>1</v>
       </c>
@@ -7890,7 +7895,7 @@
       <c r="AC1" s="33"/>
       <c r="AD1" s="33"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
@@ -7918,7 +7923,7 @@
       <c r="AC2" s="33"/>
       <c r="AD2" s="33"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
@@ -7958,7 +7963,7 @@
       <c r="AC9" s="68"/>
       <c r="AD9" s="68"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
         <v>29</v>
       </c>
@@ -8076,7 +8081,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -8193,7 +8198,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>26</v>
       </c>
@@ -8303,7 +8308,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>27</v>
       </c>
@@ -8392,7 +8397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
         <v>7</v>
       </c>
@@ -8508,7 +8513,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -8539,7 +8544,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -8569,7 +8574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -8607,7 +8612,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -8636,7 +8641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="C19"/>
       <c r="AC19" s="32" t="str">
@@ -8648,7 +8653,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="AC20" s="32" t="str">
@@ -8660,7 +8665,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="C21"/>
       <c r="AC21" s="32" t="str">
@@ -8672,7 +8677,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="C22"/>
       <c r="AC22" s="32" t="str">
@@ -8684,7 +8689,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="C23"/>
       <c r="AC23" s="32" t="str">
@@ -8696,7 +8701,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="C24"/>
       <c r="AC24" s="32" t="str">
@@ -8708,11 +8713,11 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="C26"/>
       <c r="AC26" s="32" t="str">
@@ -8724,7 +8729,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="C27"/>
       <c r="AC27" s="32" t="str">
@@ -8736,7 +8741,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="C28"/>
       <c r="AC28" s="32" t="str">
@@ -8748,7 +8753,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="C29"/>
       <c r="AC29" s="32" t="str">
@@ -8760,7 +8765,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="C30"/>
       <c r="AC30" s="32" t="str">
@@ -8772,7 +8777,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="C31"/>
       <c r="AC31" s="32" t="str">
@@ -8784,7 +8789,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="C32"/>
       <c r="AC32" s="32" t="str">
@@ -8796,7 +8801,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="C33"/>
       <c r="AC33" s="32" t="str">
@@ -8808,7 +8813,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="C34"/>
       <c r="AC34" s="32" t="str">
@@ -8820,11 +8825,11 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="C36"/>
       <c r="AC36" s="32" t="str">
@@ -8836,7 +8841,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="C37"/>
       <c r="AC37" s="32" t="str">
@@ -8848,7 +8853,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="C38"/>
       <c r="AC38" s="32" t="str">
@@ -8860,7 +8865,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="C39"/>
       <c r="AC39" s="32" t="str">
@@ -8872,7 +8877,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="C40"/>
       <c r="AC40" s="32" t="str">
@@ -8884,7 +8889,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
       <c r="C41"/>
       <c r="D41" s="33" t="str">
@@ -8904,7 +8909,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C42"/>
       <c r="D42" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8923,7 +8928,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C43"/>
       <c r="D43" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8942,7 +8947,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C44"/>
       <c r="D44" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8961,7 +8966,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C45"/>
       <c r="D45" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8980,7 +8985,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C46"/>
       <c r="D46" s="33" t="str">
         <f t="shared" si="6"/>
@@ -8999,7 +9004,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C47"/>
       <c r="D47" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9018,7 +9023,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C48"/>
       <c r="D48" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9037,7 +9042,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49"/>
       <c r="D49" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9056,7 +9061,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50"/>
       <c r="D50" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9075,7 +9080,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51"/>
       <c r="D51" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9094,7 +9099,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52"/>
       <c r="D52" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9113,7 +9118,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53"/>
       <c r="D53" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9132,7 +9137,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54"/>
       <c r="D54" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9151,7 +9156,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C55"/>
       <c r="D55" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9170,7 +9175,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56"/>
       <c r="D56" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9189,7 +9194,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57"/>
       <c r="D57" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9208,7 +9213,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C58"/>
       <c r="D58" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9227,7 +9232,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C59"/>
       <c r="D59" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9246,7 +9251,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C60"/>
       <c r="D60" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9265,7 +9270,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C61"/>
       <c r="D61" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9284,7 +9289,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C62"/>
       <c r="D62" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9391,7 +9396,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C63"/>
       <c r="D63" s="33" t="str">
         <f t="shared" si="6"/>
@@ -9498,80 +9503,80 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.15">
+    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C64"/>
       <c r="D64" s="33" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87"/>
     </row>
   </sheetData>
@@ -9614,13 +9619,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>2311400</xdr:colOff>
+                    <xdr:colOff>2308860</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9636,13 +9641,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2590800</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9665,7 +9670,7 @@
       <selection pane="bottomLeft" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
@@ -9674,11 +9679,11 @@
     <col min="5" max="5" width="6.33203125" style="2" customWidth="1"/>
     <col min="6" max="30" width="4.33203125" style="2" customWidth="1"/>
     <col min="31" max="31" width="8.6640625" customWidth="1"/>
-    <col min="32" max="32" width="45.1640625" customWidth="1"/>
+    <col min="32" max="32" width="45.109375" customWidth="1"/>
     <col min="33" max="256" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="30">
         <v>1</v>
       </c>
@@ -9710,7 +9715,7 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -9738,7 +9743,7 @@
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>12</v>
       </c>
@@ -9778,7 +9783,7 @@
       <c r="AC9" s="21"/>
       <c r="AD9" s="21"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>29</v>
       </c>
@@ -9896,7 +9901,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -10012,7 +10017,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>26</v>
       </c>
@@ -10122,7 +10127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>27</v>
       </c>
@@ -10211,7 +10216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>7</v>
       </c>
@@ -10327,7 +10332,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" ht="39.6" x14ac:dyDescent="0.25">
       <c r="D15" t="str">
         <f t="shared" ref="D15:D59" si="4">IF(A15&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10340,7 +10345,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D16" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10358,7 +10363,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="17" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D17" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10376,7 +10381,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="18" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D18" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10394,7 +10399,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="19" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D19" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10412,7 +10417,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="20" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D20" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10430,7 +10435,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="21" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D21" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10448,7 +10453,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="22" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
         <f>IF(A22&lt;&gt;"","Planned","")</f>
         <v/>
@@ -10466,7 +10471,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10484,7 +10489,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="24" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D24" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10502,7 +10507,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D25" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10520,7 +10525,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="26" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D26" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10538,7 +10543,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="27" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D27" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10556,7 +10561,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D28" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10574,7 +10579,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D29" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10592,7 +10597,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D30" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10610,7 +10615,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D31" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10628,7 +10633,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D32" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10646,7 +10651,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="33" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D33" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10664,7 +10669,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="34" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D34" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10682,7 +10687,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="35" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D35" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10700,7 +10705,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="36" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D36" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10718,7 +10723,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="37" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D37" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10736,7 +10741,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="38" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D38" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10754,7 +10759,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="39" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D39" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10772,7 +10777,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="40" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D40" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10790,7 +10795,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="41" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D41" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10808,7 +10813,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="42" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D42" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10826,7 +10831,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="43" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D43" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10844,7 +10849,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="44" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D44" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10862,7 +10867,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="45" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D45" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10880,7 +10885,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="46" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D46" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10898,7 +10903,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="47" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D47" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10916,7 +10921,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="48" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D48" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10934,7 +10939,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="49" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D49" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10952,7 +10957,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="50" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D50" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10970,7 +10975,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="51" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D51" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -10988,7 +10993,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="52" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D52" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11006,7 +11011,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="53" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D53" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11024,7 +11029,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="54" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D54" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11042,7 +11047,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="55" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D55" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11060,7 +11065,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="56" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D56" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11078,7 +11083,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="57" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D57" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11096,7 +11101,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="58" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D58" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11202,7 +11207,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="59" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D59" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -11308,7 +11313,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="4:30" x14ac:dyDescent="0.15">
+    <row r="64" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D64" t="str">
         <f>IF(A64&lt;&gt;"","Planned","")</f>
         <v/>
@@ -11362,13 +11367,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>266700</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>1981200</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11384,13 +11389,13 @@
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>2286000</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>254000</xdr:colOff>
+                    <xdr:colOff>251460</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11414,18 +11419,18 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.1640625" style="33"/>
+    <col min="1" max="3" width="9.109375" style="33"/>
     <col min="4" max="4" width="32.6640625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="33"/>
+    <col min="5" max="5" width="9.109375" style="33"/>
     <col min="6" max="6" width="32.6640625" style="33" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="33"/>
+    <col min="7" max="7" width="9.109375" style="33"/>
     <col min="8" max="8" width="41.6640625" style="33" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="33"/>
+    <col min="9" max="16384" width="9.109375" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
         <v>95</v>
       </c>
@@ -11441,7 +11446,7 @@
       <c r="E1" s="81"/>
       <c r="F1" s="82"/>
     </row>
-    <row r="2" spans="1:8" ht="42" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="83" t="s">
         <v>97</v>
       </c>
@@ -11456,7 +11461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="85"/>
       <c r="B3" s="77"/>
       <c r="C3" s="77"/>
@@ -11464,7 +11469,7 @@
       <c r="E3" s="77"/>
       <c r="F3" s="86"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="87"/>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
@@ -11472,7 +11477,7 @@
       <c r="E4" s="78"/>
       <c r="F4" s="88"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C15)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11483,7 +11488,7 @@
       <c r="E5" s="75"/>
       <c r="F5" s="94"/>
     </row>
-    <row r="6" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="89" t="s">
         <v>94</v>
       </c>
@@ -11499,8 +11504,8 @@
       </c>
       <c r="F6" s="92"/>
     </row>
-    <row r="8" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
         <v>95</v>
       </c>
@@ -11516,7 +11521,7 @@
       <c r="E9" s="81"/>
       <c r="F9" s="82"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="83" t="s">
         <v>97</v>
       </c>
@@ -11528,7 +11533,7 @@
       <c r="E10" s="76"/>
       <c r="F10" s="84"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="85"/>
       <c r="B11" s="77"/>
       <c r="C11" s="77"/>
@@ -11536,7 +11541,7 @@
       <c r="E11" s="77"/>
       <c r="F11" s="86"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="87"/>
       <c r="B12" s="78"/>
       <c r="C12" s="78"/>
@@ -11544,7 +11549,7 @@
       <c r="E12" s="78"/>
       <c r="F12" s="88"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C16)</f>
         <v>Responsible Person: Tina Tester</v>
@@ -11555,7 +11560,7 @@
       <c r="E13" s="75"/>
       <c r="F13" s="94"/>
     </row>
-    <row r="14" spans="1:8" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="89" t="s">
         <v>94</v>
       </c>
@@ -11571,8 +11576,8 @@
       </c>
       <c r="F14" s="92"/>
     </row>
-    <row r="16" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
         <v>95</v>
       </c>
@@ -11588,7 +11593,7 @@
       <c r="E17" s="81"/>
       <c r="F17" s="82"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
         <v>97</v>
       </c>
@@ -11600,7 +11605,7 @@
       <c r="E18" s="76"/>
       <c r="F18" s="84"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="85"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77"/>
@@ -11608,7 +11613,7 @@
       <c r="E19" s="77"/>
       <c r="F19" s="86"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="87"/>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
@@ -11616,7 +11621,7 @@
       <c r="E20" s="78"/>
       <c r="F20" s="88"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C17)</f>
         <v>Responsible Person: Danny Dev</v>
@@ -11627,7 +11632,7 @@
       <c r="E21" s="75"/>
       <c r="F21" s="94"/>
     </row>
-    <row r="22" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="89" t="s">
         <v>94</v>
       </c>
@@ -11643,8 +11648,8 @@
       </c>
       <c r="F22" s="92"/>
     </row>
-    <row r="24" spans="1:6" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
         <v>95</v>
       </c>
@@ -11660,7 +11665,7 @@
       <c r="E25" s="81"/>
       <c r="F25" s="82"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
         <v>97</v>
       </c>
@@ -11672,7 +11677,7 @@
       <c r="E26" s="76"/>
       <c r="F26" s="84"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="85"/>
       <c r="B27" s="77"/>
       <c r="C27" s="77"/>
@@ -11680,7 +11685,7 @@
       <c r="E27" s="77"/>
       <c r="F27" s="86"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="87"/>
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
@@ -11688,7 +11693,7 @@
       <c r="E28" s="78"/>
       <c r="F28" s="88"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="93" t="str">
         <f>CONCATENATE("Responsible Person: ",'Sp1'!C18)</f>
         <v xml:space="preserve">Responsible Person: </v>
@@ -11699,7 +11704,7 @@
       <c r="E29" s="75"/>
       <c r="F29" s="94"/>
     </row>
-    <row r="30" spans="1:6" ht="29" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="89" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Updated SCRUM spreadsheet for sprint 3
</commit_message>
<xml_diff>
--- a/INFO310 Project Management.xlsx
+++ b/INFO310 Project Management.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\__INFO310\SubscriptionTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CACCB58-AC24-488E-A986-D23D58E2DCC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC1554-B676-4DE4-B97F-11138B82608E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Plan" sheetId="7" r:id="rId1"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="133">
   <si>
     <t>Goal</t>
   </si>
@@ -326,9 +326,6 @@
   </si>
   <si>
     <t>Size</t>
-  </si>
-  <si>
-    <t>Planned</t>
   </si>
   <si>
     <t>Unallocated stories</t>
@@ -697,6 +694,12 @@
   </si>
   <si>
     <t xml:space="preserve">As a contractor I want to be able to securely log in so that I can protect my clients data </t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Removed</t>
   </si>
 </sst>
 </file>
@@ -2005,16 +2008,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2098,16 +2101,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>294.66666666666663</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>239.66666666666663</c:v>
+                  <c:v>227.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>184.66666666666663</c:v>
+                  <c:v>174.99999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>129.66666666666663</c:v>
+                  <c:v>122.49999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2488,6 +2491,9 @@
                 <c:pt idx="1">
                   <c:v>21</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2536,13 +2542,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2578,13 +2584,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2620,13 +2626,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>64.666666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4876,8 +4882,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4906,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="45" t="s">
         <v>2</v>
@@ -5071,7 +5077,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5087,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>2</v>
@@ -5105,7 +5111,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J15" s="1"/>
     </row>
@@ -5127,11 +5133,11 @@
         <v>92</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I16" s="71">
         <v>1</v>
@@ -5156,11 +5162,11 @@
         <v>102</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I17" s="37">
         <v>1</v>
@@ -5184,13 +5190,14 @@
       <c r="E18" s="22">
         <v>112</v>
       </c>
-      <c r="F18" s="4" t="str">
-        <f>IF(AND(OR(F17="Planned",F17="Ongoing"),C18&lt;&gt;""),"Planned","Unplanned")</f>
-        <v>Planned</v>
-      </c>
-      <c r="G18" s="27"/>
+      <c r="F18" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="74">
+        <v>44340</v>
+      </c>
       <c r="H18" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I18" s="37">
         <v>1</v>
@@ -5453,7 +5460,7 @@
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
       <c r="D31" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" s="25">
         <f>SUMIF('Product Backlog'!E$25:E$103,"",'Product Backlog'!D$25:D$103)-SUMIF('Product Backlog'!C$25:C$103,"Removed",'Product Backlog'!D$25:D$103)</f>
@@ -5511,8 +5518,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5530,7 +5537,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5538,7 +5545,7 @@
     </row>
     <row r="4" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>6</v>
@@ -5553,10 +5560,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="106.2" thickBot="1" x14ac:dyDescent="0.3">
@@ -5564,10 +5571,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="111" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="107" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="106">
         <v>34</v>
@@ -5576,13 +5583,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G5" s="111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
@@ -5590,10 +5597,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="108" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="108">
         <v>5</v>
@@ -5602,7 +5609,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="110"/>
       <c r="I6" s="31">
@@ -5615,10 +5622,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="103">
         <v>13</v>
@@ -5627,7 +5634,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="66" x14ac:dyDescent="0.25">
@@ -5635,10 +5642,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="103">
         <v>2</v>
@@ -5647,7 +5654,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="97"/>
     </row>
@@ -5656,10 +5663,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D9" s="103">
         <v>3</v>
@@ -5668,7 +5675,7 @@
         <v>44198</v>
       </c>
       <c r="F9" s="113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -5676,10 +5683,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="103" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D10" s="103">
         <v>2</v>
@@ -5688,10 +5695,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G10" s="97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5699,10 +5706,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D11" s="103">
         <v>8</v>
@@ -5711,7 +5718,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
@@ -5719,10 +5726,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D12" s="103">
         <v>13</v>
@@ -5731,10 +5738,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G12" s="97" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
@@ -5742,10 +5749,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D13" s="103">
         <v>21</v>
@@ -5754,7 +5761,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
@@ -5762,10 +5769,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="98" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="98">
         <v>8</v>
@@ -5774,7 +5781,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="114" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G14" s="100"/>
     </row>
@@ -5783,10 +5790,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="103" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D15" s="103">
         <v>55</v>
@@ -5795,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
@@ -5803,10 +5810,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="103">
         <v>13</v>
@@ -5815,7 +5822,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
@@ -5823,10 +5830,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="97" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="103" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D17" s="103">
         <v>55</v>
@@ -5835,7 +5842,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
@@ -5843,10 +5850,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="97" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="103">
         <v>1</v>
@@ -5855,10 +5862,10 @@
         <v>1</v>
       </c>
       <c r="F18" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="97" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
@@ -5866,10 +5873,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="97" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D19" s="103">
         <v>12</v>
@@ -5878,10 +5885,10 @@
         <v>2</v>
       </c>
       <c r="F19" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G19" s="97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
@@ -5889,10 +5896,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="97" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="103">
         <v>1</v>
@@ -5901,7 +5908,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
@@ -5909,10 +5916,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="97" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="103" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D21" s="103">
         <v>12</v>
@@ -5921,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="100" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
@@ -5929,10 +5936,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="97" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" s="103" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="D22" s="103">
         <v>15</v>
@@ -5941,7 +5948,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G22" s="31"/>
     </row>
@@ -5950,10 +5957,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="103">
         <v>21</v>
@@ -5962,7 +5969,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
@@ -5970,10 +5977,10 @@
         <v>20</v>
       </c>
       <c r="B24" s="97" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="103" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="103">
         <v>12</v>
@@ -5982,7 +5989,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
@@ -6084,8 +6091,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="96" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A13" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6106,18 +6113,18 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>306</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="52">
         <f>IF(COUNT(B28:B39)=0,1,COUNT(B28:B39))</f>
@@ -6126,58 +6133,58 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="52">
         <f>IF(COUNT(D28:D51)=0,1,COUNT(D28:D51)+1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="52">
         <f>IF(G4&gt;D4,G4-D4,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="52">
         <f>TrendSprintCount-TrendOffset</f>
         <v>3</v>
       </c>
       <c r="Z6" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="Z7" s="36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -6188,83 +6195,83 @@
       <c r="B8" s="118"/>
       <c r="D8" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,TrendOffset,0,SprintsInTrend,1)))</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Z8" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="55">
         <f ca="1">IF(D28="","",AVERAGE(OFFSET(D27,1,0,SprintCount,1)))</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="52">
         <f ca="1">IF(M28="",1,COUNT(M28:M110))</f>
         <v>4</v>
       </c>
       <c r="Z9" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="55">
         <f ca="1">IF(D28="","",AVERAGE(LastEight))</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Z10" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="55">
         <f ca="1">IF(D28="","",IF(TrendSprintCount&lt;4,D10,AVERAGE(SMALL(LastEight,1),SMALL(LastEight,2),SMALL(LastEight,3))))</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Z11" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="55">
         <f ca="1">IF(M29="","",M28-M29)</f>
-        <v>55</v>
+        <v>52.5</v>
       </c>
       <c r="Z12" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="F13" s="53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z13" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="56">
         <f>IF(D7="",0,ROUNDUP(D3/D7*0.6,0))</f>
@@ -6273,7 +6280,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="56">
         <f>IF(D7="",0,ROUNDUP(D3/D7,0))</f>
@@ -6282,18 +6289,18 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="56">
         <f>IF(D7="",0,ROUNDUP(D3/D7*1.6,0))</f>
         <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17">
         <f>IF(OR(D28="",D29=""),1,STDEV(D28:D51))</f>
-        <v>48.083261120685229</v>
+        <v>37.898988552906438</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -6304,19 +6311,19 @@
       <c r="B18" s="118"/>
       <c r="D18" s="56">
         <f ca="1">IF(D8="","",IF(LastRealized="",ROUNDUP(LastPlanned/D8,0)+SprintCount-1,ROUNDUP((LastPlanned-LastRealized)/D8+SprintCount,0)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/D9+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D9,0)+SprintCount))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19">
         <f ca="1">LastPlanned</f>
@@ -6325,32 +6332,32 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="56">
         <f ca="1">IF(D10="","",IF(LastRealized="",ROUNDUP(LastPlanned/D10+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D10,0)+SprintCount))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20">
         <f ca="1">LastRealized</f>
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="56">
         <f ca="1">IF(D11="","",IF(LastRealized="",ROUNDUP(LastPlanned/D11+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/D11,0)+SprintCount))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="56">
         <f ca="1">IF(COUNT(M28:M51)-1&gt;0,COUNT(M28:M51)-1,"")</f>
@@ -6359,25 +6366,25 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9+G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9+G17)+SprintCount,0)))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" s="56">
         <f ca="1">IF(D9="","",IF(LastRealized="",ROUNDUP(LastPlanned/(D9-G17)+SprintCount-1,0),ROUNDUP((LastPlanned-LastRealized)/(D9-G17)+SprintCount,0)))</f>
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="120" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="120"/>
       <c r="H26" s="120"/>
@@ -6388,7 +6395,7 @@
       <c r="M26" s="120"/>
       <c r="N26" s="120"/>
       <c r="O26" s="120" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P26" s="120"/>
       <c r="Q26" s="120"/>
@@ -6398,48 +6405,48 @@
         <v>13</v>
       </c>
       <c r="B27" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="D27" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="E27" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="59" t="s">
-        <v>68</v>
-      </c>
       <c r="F27" s="60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="119" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="119"/>
       <c r="I27" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J27" s="61"/>
       <c r="K27" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L27" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M27" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N27" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O27" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P27" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q27" s="60" t="s">
         <v>70</v>
-      </c>
-      <c r="Q27" s="60" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -6481,27 +6488,27 @@
       </c>
       <c r="L28" s="52">
         <f t="shared" ref="L28:L51" ca="1" si="3">IF(TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28)&lt;N28,N28,TREND(OFFSET($K$27,TrendOffset+1,0,SprintsInTrend,1),OFFSET($A$27,TrendOffset+1,0,SprintsInTrend,1),A28))</f>
-        <v>294.66666666666663</v>
+        <v>280</v>
       </c>
       <c r="M28" s="52">
         <f ca="1">L28</f>
-        <v>294.66666666666663</v>
+        <v>280</v>
       </c>
       <c r="N28" s="52">
         <f t="shared" ref="N28:N51" ca="1" si="4">OFFSET($I$27,TrendSprintCount,0,1,1)</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O28" s="63">
         <f t="shared" ref="O28:O51" ca="1" si="5">D$9</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P28" s="63">
         <f t="shared" ref="P28:P51" ca="1" si="6">D$10</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q28" s="63">
         <f t="shared" ref="Q28:Q51" ca="1" si="7">D$11</f>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -6544,27 +6551,27 @@
       </c>
       <c r="L29" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>239.66666666666663</v>
+        <v>227.5</v>
       </c>
       <c r="M29" s="52">
         <f ca="1">IF(L29=L28,"",L29)</f>
-        <v>239.66666666666663</v>
+        <v>227.5</v>
       </c>
       <c r="N29" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O29" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P29" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q29" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -6578,7 +6585,9 @@
       <c r="C30" s="2">
         <v>114</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>84</v>
+      </c>
       <c r="E30" s="54">
         <f>IF(B30="","",IF(D29="",E29,B30+SUM(D$28:D29)))</f>
         <v>306</v>
@@ -6605,27 +6614,27 @@
       </c>
       <c r="L30" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>184.66666666666663</v>
+        <v>174.99999999999997</v>
       </c>
       <c r="M30" s="52">
         <f t="shared" ref="M30:M51" ca="1" si="10">IF(L30=L29,"",L30)</f>
-        <v>184.66666666666663</v>
+        <v>174.99999999999997</v>
       </c>
       <c r="N30" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O30" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P30" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q30" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -6639,49 +6648,49 @@
         <f>IF(B31="","",IF(D30="",E30,B31+SUM(D$28:D30)))</f>
         <v/>
       </c>
-      <c r="F31" s="52" t="str">
+      <c r="F31" s="52">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="G31" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="G31" s="52">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H31" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="H31" s="52">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I31" s="52" t="str">
+        <v>112</v>
+      </c>
+      <c r="I31" s="52">
         <f>IF(B31="",IF(B30="","",IF(D30="","",F30-D30)),IF(AND(C30="",D30=""),"",IF(AND(D30="",C30&lt;&gt;""),IF(I30&gt;F30,I30-C30,F30-C30),B$28-B31-SUM(D$28:D30))))</f>
-        <v/>
-      </c>
-      <c r="K31" t="str">
+        <v>112</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="2"/>
-        <v/>
+        <v>112</v>
       </c>
       <c r="L31" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>129.66666666666663</v>
+        <v>122.49999999999997</v>
       </c>
       <c r="M31" s="52">
         <f t="shared" ca="1" si="10"/>
-        <v>129.66666666666663</v>
+        <v>122.49999999999997</v>
       </c>
       <c r="N31" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O31" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P31" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q31" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -6726,19 +6735,19 @@
       </c>
       <c r="N32" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O32" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P32" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q32" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -6783,19 +6792,19 @@
       </c>
       <c r="N33" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O33" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P33" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q33" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -6840,19 +6849,19 @@
       </c>
       <c r="N34" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O34" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P34" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q34" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -6897,19 +6906,19 @@
       </c>
       <c r="N35" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O35" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P35" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q35" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -6954,19 +6963,19 @@
       </c>
       <c r="N36" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O36" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P36" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q36" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -7011,19 +7020,19 @@
       </c>
       <c r="N37" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O37" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P37" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q37" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -7068,19 +7077,19 @@
       </c>
       <c r="N38" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O38" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P38" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q38" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -7125,19 +7134,19 @@
       </c>
       <c r="N39" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O39" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P39" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q39" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -7181,19 +7190,19 @@
       </c>
       <c r="N40" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O40" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P40" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q40" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -7237,19 +7246,19 @@
       </c>
       <c r="N41" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O41" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P41" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q41" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -7293,19 +7302,19 @@
       </c>
       <c r="N42" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O42" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P42" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q42" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -7349,19 +7358,19 @@
       </c>
       <c r="N43" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O43" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P43" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q43" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -7405,19 +7414,19 @@
       </c>
       <c r="N44" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O44" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P44" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q44" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -7461,19 +7470,19 @@
       </c>
       <c r="N45" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O45" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P45" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q45" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -7517,19 +7526,19 @@
       </c>
       <c r="N46" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O46" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P46" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q46" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -7573,19 +7582,19 @@
       </c>
       <c r="N47" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O47" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P47" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q47" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -7629,19 +7638,19 @@
       </c>
       <c r="N48" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O48" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P48" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q48" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -7685,19 +7694,19 @@
       </c>
       <c r="N49" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O49" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P49" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q49" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -7741,19 +7750,19 @@
       </c>
       <c r="N50" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O50" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P50" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q50" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -7797,19 +7806,19 @@
       </c>
       <c r="N51" s="52">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="O51" s="63">
         <f t="shared" ca="1" si="5"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="P51" s="63">
         <f t="shared" ca="1" si="6"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
       <c r="Q51" s="63">
         <f t="shared" ca="1" si="7"/>
-        <v>55</v>
+        <v>64.666666666666671</v>
       </c>
     </row>
   </sheetData>
@@ -7845,7 +7854,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AF87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AF17" sqref="AF17"/>
     </sheetView>
@@ -7965,13 +7974,13 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="67">
         <v>5</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="66" t="s">
         <v>17</v>
@@ -8083,14 +8092,14 @@
     </row>
     <row r="11" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <f>IF(COUNTA(A15:A242)=0,1,COUNTA(A15:A242))</f>
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
         <f ca="1">IF(COUNTIF(F10:AD10,"&gt;0")=0,1,COUNTIF(F10:AD10,"&gt;0"))</f>
@@ -8200,10 +8209,10 @@
     </row>
     <row r="12" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -8310,10 +8319,10 @@
     </row>
     <row r="13" spans="1:32" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2">
         <f ca="1">IF(DoneDays&gt;B10,B10,DoneDays)</f>
@@ -8402,7 +8411,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="66" t="s">
         <v>8</v>
@@ -8515,16 +8524,16 @@
     </row>
     <row r="15" spans="1:32" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="2">
         <v>5</v>
@@ -8541,21 +8550,21 @@
       </c>
       <c r="I15" s="2"/>
       <c r="AF15" s="112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2">
         <v>7</v>
@@ -8576,16 +8585,16 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2">
         <v>12</v>
@@ -8614,7 +8623,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
@@ -9665,7 +9674,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AF15" sqref="AF15"/>
     </sheetView>
@@ -9785,13 +9794,13 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="34">
         <v>5</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>17</v>
@@ -9903,14 +9912,14 @@
     </row>
     <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <f>IF(COUNTA(A15:A242)=0,1,COUNTA(A15:A242))</f>
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2">
         <f ca="1">IF(COUNTIF(F10:AD10,"&gt;0")=0,1,COUNTIF(F10:AD10,"&gt;0"))</f>
@@ -10019,11 +10028,11 @@
     </row>
     <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" s="2">
@@ -10129,11 +10138,11 @@
     </row>
     <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2">
         <f ca="1">IF(DoneDays&gt;B10,B10,DoneDays)</f>
@@ -10221,7 +10230,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>8</v>
@@ -10342,7 +10351,7 @@
         <v/>
       </c>
       <c r="AF15" s="112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -11432,33 +11441,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="95">
         <v>1</v>
       </c>
       <c r="C1" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E1" s="81"/>
       <c r="F1" s="82"/>
     </row>
     <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="76"/>
       <c r="D2" s="76"/>
       <c r="E2" s="76"/>
       <c r="F2" s="84"/>
       <c r="H2" s="112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11490,43 +11499,43 @@
     </row>
     <row r="6" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="96">
         <v>5</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="90"/>
       <c r="E6" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="92"/>
     </row>
     <row r="8" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="95">
         <v>1</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="81"/>
       <c r="F9" s="82"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="76"/>
       <c r="D10" s="76"/>
@@ -11562,43 +11571,43 @@
     </row>
     <row r="14" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="96">
         <v>7</v>
       </c>
       <c r="C14" s="91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="90"/>
       <c r="E14" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F14" s="92"/>
     </row>
     <row r="16" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="95">
         <v>2</v>
       </c>
       <c r="C17" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" s="81"/>
       <c r="F17" s="82"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="76"/>
       <c r="D18" s="76"/>
@@ -11634,43 +11643,43 @@
     </row>
     <row r="22" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="96">
         <v>12</v>
       </c>
       <c r="C22" s="91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="90"/>
       <c r="E22" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="92"/>
     </row>
     <row r="24" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" s="95">
         <v>2</v>
       </c>
       <c r="C25" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="81"/>
       <c r="F25" s="82"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="76"/>
       <c r="D26" s="76"/>
@@ -11706,17 +11715,17 @@
     </row>
     <row r="30" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30" s="96">
         <v>9</v>
       </c>
       <c r="C30" s="91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D30" s="90"/>
       <c r="E30" s="91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="92"/>
     </row>

</xml_diff>